<commit_message>
cap nhat ngay 5/12/2023 chua danh gia dong tien
</commit_message>
<xml_diff>
--- a/2023/DongTien-T11-T12.xlsx
+++ b/2023/DongTien-T11-T12.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trung.nguyenhoang/Documents/github/2023/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/Desktop/stocks/2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0179ECCC-6AA4-C846-992F-975E20CDD914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B90322C-A32A-5C4C-9D66-22D44C9C2EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17080" xr2:uid="{B7EC2610-802E-D441-AB46-76A27057AA52}"/>
   </bookViews>
@@ -524,7 +524,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -571,6 +571,50 @@
     </xf>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -937,7 +981,7 @@
   <dimension ref="A1:FU39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="EW1" activePane="topRight" state="frozen"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="FE21" sqref="FE21"/>
     </sheetView>
   </sheetViews>
@@ -980,431 +1024,431 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:177" x14ac:dyDescent="0.2">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="82" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="87" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
-      <c r="H1" s="43"/>
-      <c r="I1" s="43"/>
-      <c r="J1" s="43"/>
-      <c r="K1" s="43"/>
-      <c r="L1" s="43"/>
-      <c r="M1" s="43"/>
-      <c r="N1" s="43"/>
-      <c r="O1" s="43"/>
-      <c r="P1" s="43"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
+      <c r="I1" s="87"/>
+      <c r="J1" s="87"/>
+      <c r="K1" s="87"/>
+      <c r="L1" s="87"/>
+      <c r="M1" s="87"/>
+      <c r="N1" s="87"/>
+      <c r="O1" s="87"/>
+      <c r="P1" s="87"/>
       <c r="Q1" s="1"/>
-      <c r="R1" s="51" t="s">
+      <c r="R1" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="S1" s="51"/>
-      <c r="T1" s="51"/>
-      <c r="U1" s="51"/>
-      <c r="V1" s="51"/>
-      <c r="W1" s="51"/>
-      <c r="X1" s="51"/>
-      <c r="Y1" s="51"/>
-      <c r="Z1" s="51"/>
-      <c r="AA1" s="51"/>
-      <c r="AB1" s="51"/>
-      <c r="AC1" s="51"/>
-      <c r="AD1" s="51"/>
-      <c r="AE1" s="51"/>
-      <c r="AF1" s="51"/>
-      <c r="AG1" s="51"/>
-      <c r="AH1" s="51"/>
-      <c r="AI1" s="51"/>
-      <c r="AJ1" s="51"/>
-      <c r="AK1" s="51"/>
-      <c r="AL1" s="51"/>
-      <c r="AM1" s="51"/>
-      <c r="AN1" s="51"/>
-      <c r="AO1" s="52" t="s">
+      <c r="S1" s="95"/>
+      <c r="T1" s="95"/>
+      <c r="U1" s="95"/>
+      <c r="V1" s="95"/>
+      <c r="W1" s="95"/>
+      <c r="X1" s="95"/>
+      <c r="Y1" s="95"/>
+      <c r="Z1" s="95"/>
+      <c r="AA1" s="95"/>
+      <c r="AB1" s="95"/>
+      <c r="AC1" s="95"/>
+      <c r="AD1" s="95"/>
+      <c r="AE1" s="95"/>
+      <c r="AF1" s="95"/>
+      <c r="AG1" s="95"/>
+      <c r="AH1" s="95"/>
+      <c r="AI1" s="95"/>
+      <c r="AJ1" s="95"/>
+      <c r="AK1" s="95"/>
+      <c r="AL1" s="95"/>
+      <c r="AM1" s="95"/>
+      <c r="AN1" s="95"/>
+      <c r="AO1" s="96" t="s">
         <v>2</v>
       </c>
-      <c r="AP1" s="52"/>
-      <c r="AQ1" s="52"/>
-      <c r="AR1" s="52"/>
-      <c r="AS1" s="52"/>
-      <c r="AT1" s="52"/>
-      <c r="AU1" s="52"/>
-      <c r="AV1" s="52"/>
-      <c r="AW1" s="52"/>
-      <c r="AX1" s="52"/>
-      <c r="AY1" s="52"/>
-      <c r="AZ1" s="52"/>
-      <c r="BA1" s="52"/>
-      <c r="BB1" s="52"/>
-      <c r="BC1" s="52"/>
+      <c r="AP1" s="96"/>
+      <c r="AQ1" s="96"/>
+      <c r="AR1" s="96"/>
+      <c r="AS1" s="96"/>
+      <c r="AT1" s="96"/>
+      <c r="AU1" s="96"/>
+      <c r="AV1" s="96"/>
+      <c r="AW1" s="96"/>
+      <c r="AX1" s="96"/>
+      <c r="AY1" s="96"/>
+      <c r="AZ1" s="96"/>
+      <c r="BA1" s="96"/>
+      <c r="BB1" s="96"/>
+      <c r="BC1" s="96"/>
       <c r="BD1" s="1"/>
       <c r="BE1" s="1"/>
-      <c r="BF1" s="39" t="s">
+      <c r="BF1" s="83" t="s">
         <v>46</v>
       </c>
-      <c r="BG1" s="39"/>
-      <c r="BH1" s="39"/>
-      <c r="BI1" s="39"/>
-      <c r="BJ1" s="39"/>
-      <c r="BK1" s="39"/>
-      <c r="BL1" s="39"/>
-      <c r="BM1" s="39"/>
-      <c r="BN1" s="39"/>
-      <c r="BO1" s="39"/>
-      <c r="BP1" s="39"/>
-      <c r="BQ1" s="39"/>
-      <c r="BR1" s="39"/>
-      <c r="BS1" s="39"/>
-      <c r="BT1" s="39"/>
-      <c r="BU1" s="39"/>
-      <c r="BV1" s="39"/>
-      <c r="BW1" s="39"/>
-      <c r="BX1" s="39"/>
-      <c r="BY1" s="39"/>
-      <c r="BZ1" s="39"/>
-      <c r="CA1" s="39"/>
-      <c r="CB1" s="39"/>
+      <c r="BG1" s="83"/>
+      <c r="BH1" s="83"/>
+      <c r="BI1" s="83"/>
+      <c r="BJ1" s="83"/>
+      <c r="BK1" s="83"/>
+      <c r="BL1" s="83"/>
+      <c r="BM1" s="83"/>
+      <c r="BN1" s="83"/>
+      <c r="BO1" s="83"/>
+      <c r="BP1" s="83"/>
+      <c r="BQ1" s="83"/>
+      <c r="BR1" s="83"/>
+      <c r="BS1" s="83"/>
+      <c r="BT1" s="83"/>
+      <c r="BU1" s="83"/>
+      <c r="BV1" s="83"/>
+      <c r="BW1" s="83"/>
+      <c r="BX1" s="83"/>
+      <c r="BY1" s="83"/>
+      <c r="BZ1" s="83"/>
+      <c r="CA1" s="83"/>
+      <c r="CB1" s="83"/>
       <c r="CC1" s="1"/>
-      <c r="CD1" s="40" t="s">
+      <c r="CD1" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="CE1" s="40"/>
-      <c r="CF1" s="40"/>
-      <c r="CG1" s="40"/>
-      <c r="CH1" s="40"/>
-      <c r="CI1" s="40"/>
-      <c r="CJ1" s="40"/>
-      <c r="CK1" s="40"/>
-      <c r="CL1" s="40"/>
-      <c r="CM1" s="40"/>
-      <c r="CN1" s="40"/>
-      <c r="CO1" s="40"/>
-      <c r="CP1" s="40"/>
-      <c r="CQ1" s="40"/>
-      <c r="CR1" s="40"/>
-      <c r="CS1" s="40"/>
-      <c r="CT1" s="40"/>
-      <c r="CU1" s="40"/>
-      <c r="CV1" s="40"/>
-      <c r="CW1" s="40"/>
-      <c r="CX1" s="40"/>
-      <c r="CY1" s="40"/>
-      <c r="CZ1" s="40"/>
-      <c r="DA1" s="40"/>
-      <c r="DB1" s="40"/>
-      <c r="DC1" s="40"/>
-      <c r="DD1" s="40"/>
-      <c r="DE1" s="40"/>
-      <c r="DF1" s="40"/>
-      <c r="DG1" s="40"/>
-      <c r="DH1" s="40"/>
-      <c r="DI1" s="40"/>
-      <c r="DJ1" s="40"/>
-      <c r="DK1" s="40"/>
-      <c r="DL1" s="40"/>
-      <c r="DM1" s="40"/>
-      <c r="DN1" s="40"/>
-      <c r="DO1" s="40"/>
-      <c r="DP1" s="40"/>
+      <c r="CE1" s="84"/>
+      <c r="CF1" s="84"/>
+      <c r="CG1" s="84"/>
+      <c r="CH1" s="84"/>
+      <c r="CI1" s="84"/>
+      <c r="CJ1" s="84"/>
+      <c r="CK1" s="84"/>
+      <c r="CL1" s="84"/>
+      <c r="CM1" s="84"/>
+      <c r="CN1" s="84"/>
+      <c r="CO1" s="84"/>
+      <c r="CP1" s="84"/>
+      <c r="CQ1" s="84"/>
+      <c r="CR1" s="84"/>
+      <c r="CS1" s="84"/>
+      <c r="CT1" s="84"/>
+      <c r="CU1" s="84"/>
+      <c r="CV1" s="84"/>
+      <c r="CW1" s="84"/>
+      <c r="CX1" s="84"/>
+      <c r="CY1" s="84"/>
+      <c r="CZ1" s="84"/>
+      <c r="DA1" s="84"/>
+      <c r="DB1" s="84"/>
+      <c r="DC1" s="84"/>
+      <c r="DD1" s="84"/>
+      <c r="DE1" s="84"/>
+      <c r="DF1" s="84"/>
+      <c r="DG1" s="84"/>
+      <c r="DH1" s="84"/>
+      <c r="DI1" s="84"/>
+      <c r="DJ1" s="84"/>
+      <c r="DK1" s="84"/>
+      <c r="DL1" s="84"/>
+      <c r="DM1" s="84"/>
+      <c r="DN1" s="84"/>
+      <c r="DO1" s="84"/>
+      <c r="DP1" s="84"/>
       <c r="DQ1" s="1"/>
-      <c r="DR1" s="41" t="s">
+      <c r="DR1" s="85" t="s">
         <v>4</v>
       </c>
-      <c r="DS1" s="41"/>
-      <c r="DT1" s="41"/>
-      <c r="DU1" s="41"/>
-      <c r="DV1" s="41"/>
-      <c r="DW1" s="41"/>
-      <c r="DX1" s="41"/>
-      <c r="DY1" s="41"/>
-      <c r="DZ1" s="41"/>
-      <c r="EA1" s="41"/>
-      <c r="EB1" s="41"/>
-      <c r="EC1" s="41"/>
-      <c r="ED1" s="41"/>
-      <c r="EE1" s="41"/>
-      <c r="EF1" s="41"/>
+      <c r="DS1" s="85"/>
+      <c r="DT1" s="85"/>
+      <c r="DU1" s="85"/>
+      <c r="DV1" s="85"/>
+      <c r="DW1" s="85"/>
+      <c r="DX1" s="85"/>
+      <c r="DY1" s="85"/>
+      <c r="DZ1" s="85"/>
+      <c r="EA1" s="85"/>
+      <c r="EB1" s="85"/>
+      <c r="EC1" s="85"/>
+      <c r="ED1" s="85"/>
+      <c r="EE1" s="85"/>
+      <c r="EF1" s="85"/>
       <c r="EG1" s="1"/>
-      <c r="EH1" s="48" t="s">
+      <c r="EH1" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="EI1" s="48"/>
-      <c r="EJ1" s="48"/>
-      <c r="EK1" s="48"/>
-      <c r="EL1" s="48"/>
-      <c r="EM1" s="48"/>
-      <c r="EN1" s="48"/>
-      <c r="EO1" s="48"/>
-      <c r="EP1" s="48"/>
-      <c r="EQ1" s="48"/>
-      <c r="ER1" s="48"/>
-      <c r="ES1" s="48"/>
-      <c r="ET1" s="48"/>
-      <c r="EU1" s="48"/>
-      <c r="EV1" s="48"/>
+      <c r="EI1" s="92"/>
+      <c r="EJ1" s="92"/>
+      <c r="EK1" s="92"/>
+      <c r="EL1" s="92"/>
+      <c r="EM1" s="92"/>
+      <c r="EN1" s="92"/>
+      <c r="EO1" s="92"/>
+      <c r="EP1" s="92"/>
+      <c r="EQ1" s="92"/>
+      <c r="ER1" s="92"/>
+      <c r="ES1" s="92"/>
+      <c r="ET1" s="92"/>
+      <c r="EU1" s="92"/>
+      <c r="EV1" s="92"/>
       <c r="EW1" s="1"/>
-      <c r="EX1" s="46" t="s">
+      <c r="EX1" s="90" t="s">
         <v>6</v>
       </c>
-      <c r="EY1" s="46"/>
-      <c r="EZ1" s="46"/>
-      <c r="FA1" s="46"/>
-      <c r="FB1" s="46"/>
-      <c r="FC1" s="46"/>
-      <c r="FD1" s="46"/>
+      <c r="EY1" s="90"/>
+      <c r="EZ1" s="90"/>
+      <c r="FA1" s="90"/>
+      <c r="FB1" s="90"/>
+      <c r="FC1" s="90"/>
+      <c r="FD1" s="90"/>
       <c r="FE1" s="1"/>
-      <c r="FF1" s="49" t="s">
+      <c r="FF1" s="93" t="s">
         <v>7</v>
       </c>
-      <c r="FG1" s="49"/>
-      <c r="FH1" s="49"/>
-      <c r="FI1" s="49"/>
-      <c r="FJ1" s="49"/>
-      <c r="FK1" s="49"/>
-      <c r="FL1" s="49"/>
+      <c r="FG1" s="93"/>
+      <c r="FH1" s="93"/>
+      <c r="FI1" s="93"/>
+      <c r="FJ1" s="93"/>
+      <c r="FK1" s="93"/>
+      <c r="FL1" s="93"/>
       <c r="FM1" s="1"/>
-      <c r="FN1" s="50" t="s">
+      <c r="FN1" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="FO1" s="50"/>
-      <c r="FP1" s="50"/>
-      <c r="FQ1" s="50"/>
-      <c r="FR1" s="50"/>
-      <c r="FS1" s="50"/>
-      <c r="FT1" s="50"/>
+      <c r="FO1" s="94"/>
+      <c r="FP1" s="94"/>
+      <c r="FQ1" s="94"/>
+      <c r="FR1" s="94"/>
+      <c r="FS1" s="94"/>
+      <c r="FT1" s="94"/>
       <c r="FU1" s="1"/>
     </row>
     <row r="2" spans="1:177" x14ac:dyDescent="0.2">
-      <c r="A2" s="38"/>
-      <c r="B2" s="47" t="s">
+      <c r="A2" s="82"/>
+      <c r="B2" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="47"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47"/>
-      <c r="F2" s="47"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="91"/>
+      <c r="E2" s="91"/>
+      <c r="F2" s="91"/>
+      <c r="G2" s="91"/>
+      <c r="H2" s="91"/>
       <c r="I2" s="1"/>
-      <c r="J2" s="42" t="s">
+      <c r="J2" s="86" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="42"/>
-      <c r="L2" s="42"/>
-      <c r="M2" s="42"/>
-      <c r="N2" s="42"/>
-      <c r="O2" s="42"/>
-      <c r="P2" s="42"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="86"/>
+      <c r="M2" s="86"/>
+      <c r="N2" s="86"/>
+      <c r="O2" s="86"/>
+      <c r="P2" s="86"/>
       <c r="Q2" s="1"/>
-      <c r="R2" s="42" t="s">
+      <c r="R2" s="86" t="s">
         <v>11</v>
       </c>
-      <c r="S2" s="42"/>
-      <c r="T2" s="42"/>
-      <c r="U2" s="42"/>
-      <c r="V2" s="42"/>
-      <c r="W2" s="42"/>
-      <c r="X2" s="42"/>
+      <c r="S2" s="86"/>
+      <c r="T2" s="86"/>
+      <c r="U2" s="86"/>
+      <c r="V2" s="86"/>
+      <c r="W2" s="86"/>
+      <c r="X2" s="86"/>
       <c r="Y2" s="1"/>
-      <c r="Z2" s="42" t="s">
+      <c r="Z2" s="86" t="s">
         <v>12</v>
       </c>
-      <c r="AA2" s="42"/>
-      <c r="AB2" s="42"/>
-      <c r="AC2" s="42"/>
-      <c r="AD2" s="42"/>
-      <c r="AE2" s="42"/>
-      <c r="AF2" s="42"/>
+      <c r="AA2" s="86"/>
+      <c r="AB2" s="86"/>
+      <c r="AC2" s="86"/>
+      <c r="AD2" s="86"/>
+      <c r="AE2" s="86"/>
+      <c r="AF2" s="86"/>
       <c r="AG2" s="1"/>
-      <c r="AH2" s="42" t="s">
+      <c r="AH2" s="86" t="s">
         <v>13</v>
       </c>
-      <c r="AI2" s="42"/>
-      <c r="AJ2" s="42"/>
-      <c r="AK2" s="42"/>
-      <c r="AL2" s="42"/>
-      <c r="AM2" s="42"/>
-      <c r="AN2" s="42"/>
+      <c r="AI2" s="86"/>
+      <c r="AJ2" s="86"/>
+      <c r="AK2" s="86"/>
+      <c r="AL2" s="86"/>
+      <c r="AM2" s="86"/>
+      <c r="AN2" s="86"/>
       <c r="AO2" s="1"/>
-      <c r="AP2" s="42" t="s">
+      <c r="AP2" s="86" t="s">
         <v>14</v>
       </c>
-      <c r="AQ2" s="42"/>
-      <c r="AR2" s="42"/>
-      <c r="AS2" s="42"/>
-      <c r="AT2" s="42"/>
-      <c r="AU2" s="42"/>
-      <c r="AV2" s="42"/>
+      <c r="AQ2" s="86"/>
+      <c r="AR2" s="86"/>
+      <c r="AS2" s="86"/>
+      <c r="AT2" s="86"/>
+      <c r="AU2" s="86"/>
+      <c r="AV2" s="86"/>
       <c r="AW2" s="1"/>
-      <c r="AX2" s="44" t="s">
+      <c r="AX2" s="88" t="s">
         <v>15</v>
       </c>
-      <c r="AY2" s="44"/>
-      <c r="AZ2" s="44"/>
-      <c r="BA2" s="44"/>
-      <c r="BB2" s="44"/>
-      <c r="BC2" s="44"/>
-      <c r="BD2" s="45"/>
+      <c r="AY2" s="88"/>
+      <c r="AZ2" s="88"/>
+      <c r="BA2" s="88"/>
+      <c r="BB2" s="88"/>
+      <c r="BC2" s="88"/>
+      <c r="BD2" s="89"/>
       <c r="BE2" s="1"/>
-      <c r="BF2" s="44" t="s">
+      <c r="BF2" s="88" t="s">
         <v>16</v>
       </c>
-      <c r="BG2" s="44"/>
-      <c r="BH2" s="44"/>
-      <c r="BI2" s="44"/>
-      <c r="BJ2" s="44"/>
-      <c r="BK2" s="45"/>
+      <c r="BG2" s="88"/>
+      <c r="BH2" s="88"/>
+      <c r="BI2" s="88"/>
+      <c r="BJ2" s="88"/>
+      <c r="BK2" s="89"/>
       <c r="BL2" s="2"/>
       <c r="BM2" s="1"/>
-      <c r="BN2" s="42" t="s">
+      <c r="BN2" s="86" t="s">
         <v>17</v>
       </c>
-      <c r="BO2" s="42"/>
-      <c r="BP2" s="42"/>
-      <c r="BQ2" s="42"/>
-      <c r="BR2" s="42"/>
-      <c r="BS2" s="42"/>
-      <c r="BT2" s="42"/>
+      <c r="BO2" s="86"/>
+      <c r="BP2" s="86"/>
+      <c r="BQ2" s="86"/>
+      <c r="BR2" s="86"/>
+      <c r="BS2" s="86"/>
+      <c r="BT2" s="86"/>
       <c r="BU2" s="1"/>
-      <c r="BV2" s="42" t="s">
+      <c r="BV2" s="86" t="s">
         <v>18</v>
       </c>
-      <c r="BW2" s="42"/>
-      <c r="BX2" s="42"/>
-      <c r="BY2" s="42"/>
-      <c r="BZ2" s="42"/>
-      <c r="CA2" s="42"/>
-      <c r="CB2" s="42"/>
+      <c r="BW2" s="86"/>
+      <c r="BX2" s="86"/>
+      <c r="BY2" s="86"/>
+      <c r="BZ2" s="86"/>
+      <c r="CA2" s="86"/>
+      <c r="CB2" s="86"/>
       <c r="CC2" s="1"/>
-      <c r="CD2" s="42" t="s">
+      <c r="CD2" s="86" t="s">
         <v>19</v>
       </c>
-      <c r="CE2" s="42"/>
-      <c r="CF2" s="42"/>
-      <c r="CG2" s="42"/>
-      <c r="CH2" s="42"/>
-      <c r="CI2" s="42"/>
-      <c r="CJ2" s="42"/>
+      <c r="CE2" s="86"/>
+      <c r="CF2" s="86"/>
+      <c r="CG2" s="86"/>
+      <c r="CH2" s="86"/>
+      <c r="CI2" s="86"/>
+      <c r="CJ2" s="86"/>
       <c r="CK2" s="1"/>
-      <c r="CL2" s="42" t="s">
+      <c r="CL2" s="86" t="s">
         <v>20</v>
       </c>
-      <c r="CM2" s="42"/>
-      <c r="CN2" s="42"/>
-      <c r="CO2" s="42"/>
-      <c r="CP2" s="42"/>
-      <c r="CQ2" s="42"/>
-      <c r="CR2" s="42"/>
+      <c r="CM2" s="86"/>
+      <c r="CN2" s="86"/>
+      <c r="CO2" s="86"/>
+      <c r="CP2" s="86"/>
+      <c r="CQ2" s="86"/>
+      <c r="CR2" s="86"/>
       <c r="CS2" s="1"/>
-      <c r="CT2" s="42" t="s">
+      <c r="CT2" s="86" t="s">
         <v>21</v>
       </c>
-      <c r="CU2" s="42"/>
-      <c r="CV2" s="42"/>
-      <c r="CW2" s="42"/>
-      <c r="CX2" s="42"/>
-      <c r="CY2" s="42"/>
-      <c r="CZ2" s="42"/>
+      <c r="CU2" s="86"/>
+      <c r="CV2" s="86"/>
+      <c r="CW2" s="86"/>
+      <c r="CX2" s="86"/>
+      <c r="CY2" s="86"/>
+      <c r="CZ2" s="86"/>
       <c r="DA2" s="1"/>
-      <c r="DB2" s="42" t="s">
+      <c r="DB2" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="DC2" s="42"/>
-      <c r="DD2" s="42"/>
-      <c r="DE2" s="42"/>
-      <c r="DF2" s="42"/>
-      <c r="DG2" s="42"/>
-      <c r="DH2" s="42"/>
+      <c r="DC2" s="86"/>
+      <c r="DD2" s="86"/>
+      <c r="DE2" s="86"/>
+      <c r="DF2" s="86"/>
+      <c r="DG2" s="86"/>
+      <c r="DH2" s="86"/>
       <c r="DI2" s="1"/>
-      <c r="DJ2" s="42" t="s">
+      <c r="DJ2" s="86" t="s">
         <v>23</v>
       </c>
-      <c r="DK2" s="42"/>
-      <c r="DL2" s="42"/>
-      <c r="DM2" s="42"/>
-      <c r="DN2" s="42"/>
-      <c r="DO2" s="42"/>
-      <c r="DP2" s="42"/>
+      <c r="DK2" s="86"/>
+      <c r="DL2" s="86"/>
+      <c r="DM2" s="86"/>
+      <c r="DN2" s="86"/>
+      <c r="DO2" s="86"/>
+      <c r="DP2" s="86"/>
       <c r="DQ2" s="1"/>
-      <c r="DR2" s="42" t="s">
+      <c r="DR2" s="86" t="s">
         <v>24</v>
       </c>
-      <c r="DS2" s="42"/>
-      <c r="DT2" s="42"/>
-      <c r="DU2" s="42"/>
-      <c r="DV2" s="42"/>
-      <c r="DW2" s="42"/>
-      <c r="DX2" s="42"/>
+      <c r="DS2" s="86"/>
+      <c r="DT2" s="86"/>
+      <c r="DU2" s="86"/>
+      <c r="DV2" s="86"/>
+      <c r="DW2" s="86"/>
+      <c r="DX2" s="86"/>
       <c r="DY2" s="1"/>
-      <c r="DZ2" s="42" t="s">
+      <c r="DZ2" s="86" t="s">
         <v>25</v>
       </c>
-      <c r="EA2" s="42"/>
-      <c r="EB2" s="42"/>
-      <c r="EC2" s="42"/>
-      <c r="ED2" s="42"/>
-      <c r="EE2" s="42"/>
-      <c r="EF2" s="42"/>
+      <c r="EA2" s="86"/>
+      <c r="EB2" s="86"/>
+      <c r="EC2" s="86"/>
+      <c r="ED2" s="86"/>
+      <c r="EE2" s="86"/>
+      <c r="EF2" s="86"/>
       <c r="EG2" s="1"/>
-      <c r="EH2" s="42" t="s">
+      <c r="EH2" s="86" t="s">
         <v>26</v>
       </c>
-      <c r="EI2" s="42"/>
-      <c r="EJ2" s="42"/>
-      <c r="EK2" s="42"/>
-      <c r="EL2" s="42"/>
-      <c r="EM2" s="42"/>
-      <c r="EN2" s="42"/>
+      <c r="EI2" s="86"/>
+      <c r="EJ2" s="86"/>
+      <c r="EK2" s="86"/>
+      <c r="EL2" s="86"/>
+      <c r="EM2" s="86"/>
+      <c r="EN2" s="86"/>
       <c r="EO2" s="1"/>
-      <c r="EP2" s="42" t="s">
+      <c r="EP2" s="86" t="s">
         <v>27</v>
       </c>
-      <c r="EQ2" s="42"/>
-      <c r="ER2" s="42"/>
-      <c r="ES2" s="42"/>
-      <c r="ET2" s="42"/>
-      <c r="EU2" s="42"/>
-      <c r="EV2" s="42"/>
+      <c r="EQ2" s="86"/>
+      <c r="ER2" s="86"/>
+      <c r="ES2" s="86"/>
+      <c r="ET2" s="86"/>
+      <c r="EU2" s="86"/>
+      <c r="EV2" s="86"/>
       <c r="EW2" s="1"/>
-      <c r="EX2" s="42" t="s">
+      <c r="EX2" s="86" t="s">
         <v>28</v>
       </c>
-      <c r="EY2" s="42"/>
-      <c r="EZ2" s="42"/>
-      <c r="FA2" s="42"/>
-      <c r="FB2" s="42"/>
-      <c r="FC2" s="42"/>
-      <c r="FD2" s="42"/>
+      <c r="EY2" s="86"/>
+      <c r="EZ2" s="86"/>
+      <c r="FA2" s="86"/>
+      <c r="FB2" s="86"/>
+      <c r="FC2" s="86"/>
+      <c r="FD2" s="86"/>
       <c r="FE2" s="1"/>
-      <c r="FF2" s="42" t="s">
+      <c r="FF2" s="86" t="s">
         <v>29</v>
       </c>
-      <c r="FG2" s="42"/>
-      <c r="FH2" s="42"/>
-      <c r="FI2" s="42"/>
-      <c r="FJ2" s="42"/>
-      <c r="FK2" s="42"/>
-      <c r="FL2" s="42"/>
+      <c r="FG2" s="86"/>
+      <c r="FH2" s="86"/>
+      <c r="FI2" s="86"/>
+      <c r="FJ2" s="86"/>
+      <c r="FK2" s="86"/>
+      <c r="FL2" s="86"/>
       <c r="FM2" s="1"/>
-      <c r="FN2" s="42" t="s">
+      <c r="FN2" s="86" t="s">
         <v>30</v>
       </c>
-      <c r="FO2" s="42"/>
-      <c r="FP2" s="42"/>
-      <c r="FQ2" s="42"/>
-      <c r="FR2" s="42"/>
-      <c r="FS2" s="42"/>
-      <c r="FT2" s="42"/>
+      <c r="FO2" s="86"/>
+      <c r="FP2" s="86"/>
+      <c r="FQ2" s="86"/>
+      <c r="FR2" s="86"/>
+      <c r="FS2" s="86"/>
+      <c r="FT2" s="86"/>
       <c r="FU2" s="1"/>
     </row>
     <row r="3" spans="1:177" x14ac:dyDescent="0.2">
-      <c r="A3" s="38"/>
+      <c r="A3" s="82"/>
       <c r="B3" s="11" t="s">
         <v>32</v>
       </c>
@@ -8740,181 +8784,489 @@
       <c r="A18" s="5">
         <v>45265</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="34"/>
-      <c r="H18" s="35"/>
+      <c r="B18" s="6">
+        <v>234284</v>
+      </c>
+      <c r="C18" s="6">
+        <v>3925541</v>
+      </c>
+      <c r="D18" s="6">
+        <v>-3691257</v>
+      </c>
+      <c r="E18" s="6">
+        <v>-83351620000</v>
+      </c>
+      <c r="F18" s="6">
+        <v>27463600</v>
+      </c>
+      <c r="G18" s="38">
+        <v>0.151466850667793</v>
+      </c>
+      <c r="H18" s="39">
+        <v>-6.6518847006651251E-3</v>
+      </c>
       <c r="I18" s="1"/>
-      <c r="J18" s="6"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="6"/>
-      <c r="N18" s="6"/>
-      <c r="O18" s="34"/>
-      <c r="P18" s="35"/>
+      <c r="J18" s="6">
+        <v>580500</v>
+      </c>
+      <c r="K18" s="6">
+        <v>2602174</v>
+      </c>
+      <c r="L18" s="6">
+        <v>-2021674</v>
+      </c>
+      <c r="M18" s="6">
+        <v>-67407980000</v>
+      </c>
+      <c r="N18" s="6">
+        <v>23475502</v>
+      </c>
+      <c r="O18" s="40">
+        <v>0.13557426801778297</v>
+      </c>
+      <c r="P18" s="41">
+        <v>-1.0510510510510555E-2</v>
+      </c>
       <c r="Q18" s="1"/>
-      <c r="R18" s="6"/>
-      <c r="S18" s="6"/>
-      <c r="T18" s="6"/>
-      <c r="U18" s="6"/>
-      <c r="V18" s="6"/>
-      <c r="W18" s="34"/>
-      <c r="X18" s="35"/>
+      <c r="R18" s="6">
+        <v>60000</v>
+      </c>
+      <c r="S18" s="6">
+        <v>1234086</v>
+      </c>
+      <c r="T18" s="6">
+        <v>-1174086</v>
+      </c>
+      <c r="U18" s="6">
+        <v>-104177060000</v>
+      </c>
+      <c r="V18" s="6">
+        <v>2339861</v>
+      </c>
+      <c r="W18" s="42">
+        <v>0.55306105790044791</v>
+      </c>
+      <c r="X18" s="43">
+        <v>-7.0257611241217131E-3</v>
+      </c>
       <c r="Y18" s="1"/>
-      <c r="Z18" s="6"/>
-      <c r="AA18" s="6"/>
-      <c r="AB18" s="6"/>
-      <c r="AC18" s="6"/>
-      <c r="AD18" s="6"/>
-      <c r="AE18" s="34"/>
-      <c r="AF18" s="35"/>
+      <c r="Z18" s="6">
+        <v>1281300</v>
+      </c>
+      <c r="AA18" s="6">
+        <v>5233690</v>
+      </c>
+      <c r="AB18" s="6">
+        <v>-3952390</v>
+      </c>
+      <c r="AC18" s="6">
+        <v>-76291340000</v>
+      </c>
+      <c r="AD18" s="6">
+        <v>17250007</v>
+      </c>
+      <c r="AE18" s="44">
+        <v>0.37768042644852262</v>
+      </c>
+      <c r="AF18" s="45">
+        <v>-1.8276762402088847E-2</v>
+      </c>
       <c r="AG18" s="1"/>
-      <c r="AH18" s="6"/>
-      <c r="AI18" s="6"/>
-      <c r="AJ18" s="6"/>
-      <c r="AK18" s="6"/>
-      <c r="AL18" s="6"/>
-      <c r="AM18" s="34"/>
-      <c r="AN18" s="35"/>
+      <c r="AH18" s="6">
+        <v>151200</v>
+      </c>
+      <c r="AI18" s="6">
+        <v>1398700</v>
+      </c>
+      <c r="AJ18" s="6">
+        <v>-1247500</v>
+      </c>
+      <c r="AK18" s="6">
+        <v>-35020850000</v>
+      </c>
+      <c r="AL18" s="6">
+        <v>13499600</v>
+      </c>
+      <c r="AM18" s="46">
+        <v>0.11481080920916176</v>
+      </c>
+      <c r="AN18" s="47">
+        <v>-1.258992805755388E-2</v>
+      </c>
       <c r="AO18" s="1"/>
-      <c r="AP18" s="6"/>
-      <c r="AQ18" s="6"/>
-      <c r="AR18" s="6"/>
-      <c r="AS18" s="6"/>
-      <c r="AT18" s="6"/>
-      <c r="AU18" s="34"/>
-      <c r="AV18" s="35"/>
+      <c r="AP18" s="6">
+        <v>614100</v>
+      </c>
+      <c r="AQ18" s="6">
+        <v>7498060</v>
+      </c>
+      <c r="AR18" s="6">
+        <v>-6883960</v>
+      </c>
+      <c r="AS18" s="6">
+        <v>-188056260000</v>
+      </c>
+      <c r="AT18" s="6">
+        <v>22656100</v>
+      </c>
+      <c r="AU18" s="48">
+        <v>0.35805632920052438</v>
+      </c>
+      <c r="AV18" s="49">
+        <v>-9.1743119266055051E-3</v>
+      </c>
       <c r="AW18" s="1"/>
-      <c r="AX18" s="6"/>
-      <c r="AY18" s="6"/>
-      <c r="AZ18" s="6"/>
-      <c r="BA18" s="6"/>
-      <c r="BB18" s="6"/>
-      <c r="BC18" s="34"/>
-      <c r="BD18" s="35"/>
+      <c r="AX18" s="6">
+        <v>135700</v>
+      </c>
+      <c r="AY18" s="6">
+        <v>129600</v>
+      </c>
+      <c r="AZ18" s="6">
+        <v>6100</v>
+      </c>
+      <c r="BA18" s="6">
+        <v>159870000</v>
+      </c>
+      <c r="BB18" s="6">
+        <v>10469500</v>
+      </c>
+      <c r="BC18" s="50">
+        <v>2.5340274129614596E-2</v>
+      </c>
+      <c r="BD18" s="51">
+        <v>-1.6985138004246225E-2</v>
+      </c>
       <c r="BE18" s="1"/>
-      <c r="BF18" s="6"/>
-      <c r="BG18" s="6"/>
-      <c r="BH18" s="6"/>
-      <c r="BI18" s="6"/>
-      <c r="BJ18" s="6"/>
-      <c r="BK18" s="34"/>
-      <c r="BL18" s="35"/>
+      <c r="BF18" s="6">
+        <v>677700</v>
+      </c>
+      <c r="BG18" s="6">
+        <v>675878</v>
+      </c>
+      <c r="BH18" s="6">
+        <v>1822</v>
+      </c>
+      <c r="BI18" s="6">
+        <v>31370000</v>
+      </c>
+      <c r="BJ18" s="6">
+        <v>7196600</v>
+      </c>
+      <c r="BK18" s="52">
+        <v>0.18808576272128505</v>
+      </c>
+      <c r="BL18" s="53">
+        <v>1.2515644555693905E-3</v>
+      </c>
       <c r="BM18" s="1"/>
-      <c r="BN18" s="6"/>
-      <c r="BO18" s="6"/>
-      <c r="BP18" s="6"/>
-      <c r="BQ18" s="6"/>
-      <c r="BR18" s="6"/>
-      <c r="BS18" s="34"/>
-      <c r="BT18" s="35"/>
+      <c r="BN18" s="6">
+        <v>1816750</v>
+      </c>
+      <c r="BO18" s="6">
+        <v>2133505</v>
+      </c>
+      <c r="BP18" s="6">
+        <v>-316755</v>
+      </c>
+      <c r="BQ18" s="6">
+        <v>-7268400000</v>
+      </c>
+      <c r="BR18" s="6">
+        <v>3961100</v>
+      </c>
+      <c r="BS18" s="54">
+        <v>0.99726212415743098</v>
+      </c>
+      <c r="BT18" s="55">
+        <v>-6.5645514223194121E-3</v>
+      </c>
       <c r="BU18" s="1"/>
-      <c r="BV18" s="6"/>
-      <c r="BW18" s="6"/>
-      <c r="BX18" s="6"/>
-      <c r="BY18" s="6"/>
-      <c r="BZ18" s="6"/>
-      <c r="CA18" s="34"/>
-      <c r="CB18" s="35"/>
+      <c r="BV18" s="6">
+        <v>111900</v>
+      </c>
+      <c r="BW18" s="6">
+        <v>234902</v>
+      </c>
+      <c r="BX18" s="6">
+        <v>-123002</v>
+      </c>
+      <c r="BY18" s="6">
+        <v>-12566610000</v>
+      </c>
+      <c r="BZ18" s="6">
+        <v>414200</v>
+      </c>
+      <c r="CA18" s="56">
+        <v>0.83728150651859001</v>
+      </c>
+      <c r="CB18" s="57">
+        <v>-2.161100196463657E-2</v>
+      </c>
       <c r="CC18" s="1"/>
-      <c r="CD18" s="6"/>
-      <c r="CE18" s="6"/>
-      <c r="CF18" s="6"/>
-      <c r="CG18" s="6"/>
-      <c r="CH18" s="6"/>
-      <c r="CI18" s="34"/>
-      <c r="CJ18" s="35"/>
+      <c r="CD18" s="6">
+        <v>2325014</v>
+      </c>
+      <c r="CE18" s="6">
+        <v>6547281</v>
+      </c>
+      <c r="CF18" s="6">
+        <v>-4222267</v>
+      </c>
+      <c r="CG18" s="6">
+        <v>-172274840000</v>
+      </c>
+      <c r="CH18" s="6">
+        <v>10227900</v>
+      </c>
+      <c r="CI18" s="58">
+        <v>0.8674600846703624</v>
+      </c>
+      <c r="CJ18" s="59">
+        <v>-2.4691358024691357E-2</v>
+      </c>
       <c r="CK18" s="1"/>
-      <c r="CL18" s="6"/>
-      <c r="CM18" s="6"/>
-      <c r="CN18" s="6"/>
-      <c r="CO18" s="6"/>
-      <c r="CP18" s="6"/>
-      <c r="CQ18" s="34"/>
-      <c r="CR18" s="35"/>
+      <c r="CL18" s="6">
+        <v>253500</v>
+      </c>
+      <c r="CM18" s="6">
+        <v>3893004</v>
+      </c>
+      <c r="CN18" s="6">
+        <v>-3639504</v>
+      </c>
+      <c r="CO18" s="6">
+        <v>-76270090000</v>
+      </c>
+      <c r="CP18" s="6">
+        <v>35007200</v>
+      </c>
+      <c r="CQ18" s="60">
+        <v>0.11844717658081766</v>
+      </c>
+      <c r="CR18" s="61">
+        <v>2.179176755447956E-2</v>
+      </c>
       <c r="CS18" s="1"/>
-      <c r="CT18" s="6"/>
-      <c r="CU18" s="6"/>
-      <c r="CV18" s="6"/>
-      <c r="CW18" s="6"/>
-      <c r="CX18" s="6"/>
-      <c r="CY18" s="34"/>
-      <c r="CZ18" s="35"/>
+      <c r="CT18" s="6">
+        <v>172183</v>
+      </c>
+      <c r="CU18" s="6">
+        <v>219300</v>
+      </c>
+      <c r="CV18" s="6">
+        <v>-47117</v>
+      </c>
+      <c r="CW18" s="6">
+        <v>-1322000000</v>
+      </c>
+      <c r="CX18" s="6">
+        <v>10358600</v>
+      </c>
+      <c r="CY18" s="62">
+        <v>3.7793041530708782E-2</v>
+      </c>
+      <c r="CZ18" s="63">
+        <v>-1.6100178890876539E-2</v>
+      </c>
       <c r="DA18" s="1"/>
-      <c r="DB18" s="6"/>
-      <c r="DC18" s="6"/>
-      <c r="DD18" s="6"/>
-      <c r="DE18" s="6"/>
-      <c r="DF18" s="6"/>
-      <c r="DG18" s="34"/>
-      <c r="DH18" s="35"/>
+      <c r="DB18" s="6">
+        <v>659980</v>
+      </c>
+      <c r="DC18" s="6">
+        <v>501401</v>
+      </c>
+      <c r="DD18" s="6">
+        <v>158579</v>
+      </c>
+      <c r="DE18" s="6">
+        <v>2941910000</v>
+      </c>
+      <c r="DF18" s="6">
+        <v>39037500</v>
+      </c>
+      <c r="DG18" s="64">
+        <v>2.9750393852065321E-2</v>
+      </c>
+      <c r="DH18" s="65">
+        <v>-1.098901098901095E-2</v>
+      </c>
       <c r="DI18" s="1"/>
-      <c r="DJ18" s="6"/>
-      <c r="DK18" s="6"/>
-      <c r="DL18" s="6"/>
-      <c r="DM18" s="6"/>
-      <c r="DN18" s="6"/>
-      <c r="DO18" s="34"/>
-      <c r="DP18" s="35"/>
+      <c r="DJ18" s="6">
+        <v>635900</v>
+      </c>
+      <c r="DK18" s="6">
+        <v>281700</v>
+      </c>
+      <c r="DL18" s="6">
+        <v>354200</v>
+      </c>
+      <c r="DM18" s="6">
+        <v>11599390000</v>
+      </c>
+      <c r="DN18" s="6">
+        <v>5979300</v>
+      </c>
+      <c r="DO18" s="66">
+        <v>0.15346277992407137</v>
+      </c>
+      <c r="DP18" s="67">
+        <v>0</v>
+      </c>
       <c r="DQ18" s="1"/>
-      <c r="DR18" s="6"/>
-      <c r="DS18" s="6"/>
-      <c r="DT18" s="6"/>
-      <c r="DU18" s="6"/>
-      <c r="DV18" s="6"/>
-      <c r="DW18" s="34"/>
-      <c r="DX18" s="35"/>
+      <c r="DR18" s="6">
+        <v>62500</v>
+      </c>
+      <c r="DS18" s="6">
+        <v>155800</v>
+      </c>
+      <c r="DT18" s="6">
+        <v>-93300</v>
+      </c>
+      <c r="DU18" s="6">
+        <v>-6625120000</v>
+      </c>
+      <c r="DV18" s="6">
+        <v>948300</v>
+      </c>
+      <c r="DW18" s="68">
+        <v>0.23020141305494041</v>
+      </c>
+      <c r="DX18" s="69">
+        <v>-1.1396011396011355E-2</v>
+      </c>
       <c r="DY18" s="1"/>
-      <c r="DZ18" s="6"/>
-      <c r="EA18" s="6"/>
-      <c r="EB18" s="6"/>
-      <c r="EC18" s="6"/>
-      <c r="ED18" s="6"/>
-      <c r="EE18" s="34"/>
-      <c r="EF18" s="35"/>
+      <c r="DZ18" s="6">
+        <v>2300</v>
+      </c>
+      <c r="EA18" s="6">
+        <v>10090</v>
+      </c>
+      <c r="EB18" s="6">
+        <v>-7790</v>
+      </c>
+      <c r="EC18" s="6">
+        <v>-288210000</v>
+      </c>
+      <c r="ED18" s="6">
+        <v>3180500</v>
+      </c>
+      <c r="EE18" s="70">
+        <v>3.895613897185977E-3</v>
+      </c>
+      <c r="EF18" s="71">
+        <v>-1.2178619756427488E-2</v>
+      </c>
       <c r="EG18" s="1"/>
-      <c r="EH18" s="6"/>
-      <c r="EI18" s="6"/>
-      <c r="EJ18" s="6"/>
-      <c r="EK18" s="6"/>
-      <c r="EL18" s="6"/>
-      <c r="EM18" s="34"/>
-      <c r="EN18" s="35"/>
+      <c r="EH18" s="6">
+        <v>7500</v>
+      </c>
+      <c r="EI18" s="6">
+        <v>41200</v>
+      </c>
+      <c r="EJ18" s="6">
+        <v>-33700</v>
+      </c>
+      <c r="EK18" s="6">
+        <v>-2186870000</v>
+      </c>
+      <c r="EL18" s="6">
+        <v>1137000</v>
+      </c>
+      <c r="EM18" s="72">
+        <v>4.283201407211961E-2</v>
+      </c>
+      <c r="EN18" s="73">
+        <v>-1.7080745341614818E-2</v>
+      </c>
       <c r="EO18" s="1"/>
-      <c r="EP18" s="6"/>
-      <c r="EQ18" s="6"/>
-      <c r="ER18" s="6"/>
-      <c r="ES18" s="6"/>
-      <c r="ET18" s="6"/>
-      <c r="EU18" s="34"/>
-      <c r="EV18" s="35"/>
+      <c r="EP18" s="6">
+        <v>90200</v>
+      </c>
+      <c r="EQ18" s="6">
+        <v>258000</v>
+      </c>
+      <c r="ER18" s="6">
+        <v>-167800</v>
+      </c>
+      <c r="ES18" s="6">
+        <v>-4101900000</v>
+      </c>
+      <c r="ET18" s="6">
+        <v>11721200</v>
+      </c>
+      <c r="EU18" s="74">
+        <v>2.9706855953315361E-2</v>
+      </c>
+      <c r="EV18" s="75">
+        <v>4.0983606557377632E-3</v>
+      </c>
       <c r="EW18" s="1"/>
-      <c r="EX18" s="6"/>
-      <c r="EY18" s="6"/>
-      <c r="EZ18" s="6"/>
-      <c r="FA18" s="6"/>
-      <c r="FB18" s="6"/>
-      <c r="FC18" s="34"/>
-      <c r="FD18" s="35"/>
+      <c r="EX18" s="6">
+        <v>157400</v>
+      </c>
+      <c r="EY18" s="6">
+        <v>383421</v>
+      </c>
+      <c r="EZ18" s="6">
+        <v>-226021</v>
+      </c>
+      <c r="FA18" s="6">
+        <v>-5319820000</v>
+      </c>
+      <c r="FB18" s="6">
+        <v>28094000</v>
+      </c>
+      <c r="FC18" s="76">
+        <v>1.9250409340072612E-2</v>
+      </c>
+      <c r="FD18" s="77">
+        <v>6.410256410256502E-3</v>
+      </c>
       <c r="FE18" s="1"/>
-      <c r="FF18" s="6"/>
-      <c r="FG18" s="6"/>
-      <c r="FH18" s="6"/>
-      <c r="FI18" s="6"/>
-      <c r="FJ18" s="6"/>
-      <c r="FK18" s="34"/>
-      <c r="FL18" s="35"/>
+      <c r="FF18" s="6">
+        <v>1600</v>
+      </c>
+      <c r="FG18" s="6">
+        <v>145985</v>
+      </c>
+      <c r="FH18" s="6">
+        <v>-144385</v>
+      </c>
+      <c r="FI18" s="6">
+        <v>-14115170000</v>
+      </c>
+      <c r="FJ18" s="6">
+        <v>2049000</v>
+      </c>
+      <c r="FK18" s="78">
+        <v>7.2027818448023431E-2</v>
+      </c>
+      <c r="FL18" s="79">
+        <v>-4.1109969167523706E-3</v>
+      </c>
       <c r="FM18" s="1"/>
-      <c r="FN18" s="6"/>
-      <c r="FO18" s="6"/>
-      <c r="FP18" s="6"/>
-      <c r="FQ18" s="6"/>
-      <c r="FR18" s="6"/>
-      <c r="FS18" s="34"/>
-      <c r="FT18" s="35"/>
+      <c r="FN18" s="6">
+        <v>233200</v>
+      </c>
+      <c r="FO18" s="6">
+        <v>168400</v>
+      </c>
+      <c r="FP18" s="6">
+        <v>64800</v>
+      </c>
+      <c r="FQ18" s="6">
+        <v>4494730000</v>
+      </c>
+      <c r="FR18" s="6">
+        <v>1425500</v>
+      </c>
+      <c r="FS18" s="80">
+        <v>0.28172571027709575</v>
+      </c>
+      <c r="FT18" s="81">
+        <v>3.0478955007256808E-2</v>
+      </c>
       <c r="FU18" s="1"/>
     </row>
     <row r="19" spans="1:177" x14ac:dyDescent="0.2">
@@ -11420,19 +11772,19 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="13"/>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="97" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
+      <c r="J1" s="97"/>
+      <c r="K1" s="97"/>
+      <c r="L1" s="97"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">

</xml_diff>

<commit_message>
cap nhat du lieu 06/12
</commit_message>
<xml_diff>
--- a/2023/DongTien-T11-T12.xlsx
+++ b/2023/DongTien-T11-T12.xlsx
@@ -1,21 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/Desktop/stocks/2023/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trung.nguyenhoang/stocks/2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B90322C-A32A-5C4C-9D66-22D44C9C2EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10CE1756-954E-5D4F-A056-1C3033B00A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17080" xr2:uid="{B7EC2610-802E-D441-AB46-76A27057AA52}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17060" xr2:uid="{B7EC2610-802E-D441-AB46-76A27057AA52}"/>
   </bookViews>
   <sheets>
     <sheet name="GDNN T11-T12" sheetId="1" r:id="rId1"/>
     <sheet name="VNINDEX T11-T12" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.4" hidden="1">'GDNN T11-T12'!$A$4:$A$19</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'GDNN T11-T12'!$B$4:$B$19</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'GDNN T11-T12'!$C$4:$C$19</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'GDNN T11-T12'!$D$4:$D$19</definedName>
+    <definedName name="_xlchart.v2.0" hidden="1">'GDNN T11-T12'!$A$4:$A$19</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">'GDNN T11-T12'!$B$4:$B$19</definedName>
+    <definedName name="_xlchart.v2.2" hidden="1">'GDNN T11-T12'!$C$4:$C$19</definedName>
+    <definedName name="_xlchart.v2.3" hidden="1">'GDNN T11-T12'!$D$4:$D$19</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="76">
   <si>
     <t>CHỨNG KHOÁN</t>
   </si>
@@ -195,9 +205,6 @@
     <t>NN GT Mua - Bán</t>
   </si>
   <si>
-    <t>NN KL Mua - Bán</t>
-  </si>
-  <si>
     <t>Khối lượng</t>
   </si>
   <si>
@@ -220,9 +227,6 @@
   </si>
   <si>
     <t>Biên độ TB</t>
-  </si>
-  <si>
-    <t>Luỹ kế giá trị mua bán của NN</t>
   </si>
   <si>
     <t>12.21%</t>
@@ -268,6 +272,9 @@
   </si>
   <si>
     <t>Luỹ kế biến động VNI</t>
+  </si>
+  <si>
+    <t>Luỹ kế GTGD của NN</t>
   </si>
 </sst>
 </file>
@@ -524,7 +531,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -571,50 +578,27 @@
     </xf>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -627,42 +611,20 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -982,13 +944,14 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="FE21" sqref="FE21"/>
+      <selection pane="topRight" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" customWidth="1"/>
+    <col min="1" max="1" width="22" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5" customWidth="1"/>
     <col min="5" max="5" width="15.6640625" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
@@ -1024,431 +987,431 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:177" x14ac:dyDescent="0.2">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="87" t="s">
+      <c r="B1" s="53" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="F1" s="87"/>
-      <c r="G1" s="87"/>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
-      <c r="K1" s="87"/>
-      <c r="L1" s="87"/>
-      <c r="M1" s="87"/>
-      <c r="N1" s="87"/>
-      <c r="O1" s="87"/>
-      <c r="P1" s="87"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
+      <c r="N1" s="53"/>
+      <c r="O1" s="53"/>
+      <c r="P1" s="53"/>
       <c r="Q1" s="1"/>
-      <c r="R1" s="95" t="s">
+      <c r="R1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="S1" s="95"/>
-      <c r="T1" s="95"/>
-      <c r="U1" s="95"/>
-      <c r="V1" s="95"/>
-      <c r="W1" s="95"/>
-      <c r="X1" s="95"/>
-      <c r="Y1" s="95"/>
-      <c r="Z1" s="95"/>
-      <c r="AA1" s="95"/>
-      <c r="AB1" s="95"/>
-      <c r="AC1" s="95"/>
-      <c r="AD1" s="95"/>
-      <c r="AE1" s="95"/>
-      <c r="AF1" s="95"/>
-      <c r="AG1" s="95"/>
-      <c r="AH1" s="95"/>
-      <c r="AI1" s="95"/>
-      <c r="AJ1" s="95"/>
-      <c r="AK1" s="95"/>
-      <c r="AL1" s="95"/>
-      <c r="AM1" s="95"/>
-      <c r="AN1" s="95"/>
-      <c r="AO1" s="96" t="s">
+      <c r="S1" s="41"/>
+      <c r="T1" s="41"/>
+      <c r="U1" s="41"/>
+      <c r="V1" s="41"/>
+      <c r="W1" s="41"/>
+      <c r="X1" s="41"/>
+      <c r="Y1" s="41"/>
+      <c r="Z1" s="41"/>
+      <c r="AA1" s="41"/>
+      <c r="AB1" s="41"/>
+      <c r="AC1" s="41"/>
+      <c r="AD1" s="41"/>
+      <c r="AE1" s="41"/>
+      <c r="AF1" s="41"/>
+      <c r="AG1" s="41"/>
+      <c r="AH1" s="41"/>
+      <c r="AI1" s="41"/>
+      <c r="AJ1" s="41"/>
+      <c r="AK1" s="41"/>
+      <c r="AL1" s="41"/>
+      <c r="AM1" s="41"/>
+      <c r="AN1" s="41"/>
+      <c r="AO1" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="AP1" s="96"/>
-      <c r="AQ1" s="96"/>
-      <c r="AR1" s="96"/>
-      <c r="AS1" s="96"/>
-      <c r="AT1" s="96"/>
-      <c r="AU1" s="96"/>
-      <c r="AV1" s="96"/>
-      <c r="AW1" s="96"/>
-      <c r="AX1" s="96"/>
-      <c r="AY1" s="96"/>
-      <c r="AZ1" s="96"/>
-      <c r="BA1" s="96"/>
-      <c r="BB1" s="96"/>
-      <c r="BC1" s="96"/>
+      <c r="AP1" s="42"/>
+      <c r="AQ1" s="42"/>
+      <c r="AR1" s="42"/>
+      <c r="AS1" s="42"/>
+      <c r="AT1" s="42"/>
+      <c r="AU1" s="42"/>
+      <c r="AV1" s="42"/>
+      <c r="AW1" s="42"/>
+      <c r="AX1" s="42"/>
+      <c r="AY1" s="42"/>
+      <c r="AZ1" s="42"/>
+      <c r="BA1" s="42"/>
+      <c r="BB1" s="42"/>
+      <c r="BC1" s="42"/>
       <c r="BD1" s="1"/>
       <c r="BE1" s="1"/>
-      <c r="BF1" s="83" t="s">
+      <c r="BF1" s="46" t="s">
         <v>46</v>
       </c>
-      <c r="BG1" s="83"/>
-      <c r="BH1" s="83"/>
-      <c r="BI1" s="83"/>
-      <c r="BJ1" s="83"/>
-      <c r="BK1" s="83"/>
-      <c r="BL1" s="83"/>
-      <c r="BM1" s="83"/>
-      <c r="BN1" s="83"/>
-      <c r="BO1" s="83"/>
-      <c r="BP1" s="83"/>
-      <c r="BQ1" s="83"/>
-      <c r="BR1" s="83"/>
-      <c r="BS1" s="83"/>
-      <c r="BT1" s="83"/>
-      <c r="BU1" s="83"/>
-      <c r="BV1" s="83"/>
-      <c r="BW1" s="83"/>
-      <c r="BX1" s="83"/>
-      <c r="BY1" s="83"/>
-      <c r="BZ1" s="83"/>
-      <c r="CA1" s="83"/>
-      <c r="CB1" s="83"/>
+      <c r="BG1" s="46"/>
+      <c r="BH1" s="46"/>
+      <c r="BI1" s="46"/>
+      <c r="BJ1" s="46"/>
+      <c r="BK1" s="46"/>
+      <c r="BL1" s="46"/>
+      <c r="BM1" s="46"/>
+      <c r="BN1" s="46"/>
+      <c r="BO1" s="46"/>
+      <c r="BP1" s="46"/>
+      <c r="BQ1" s="46"/>
+      <c r="BR1" s="46"/>
+      <c r="BS1" s="46"/>
+      <c r="BT1" s="46"/>
+      <c r="BU1" s="46"/>
+      <c r="BV1" s="46"/>
+      <c r="BW1" s="46"/>
+      <c r="BX1" s="46"/>
+      <c r="BY1" s="46"/>
+      <c r="BZ1" s="46"/>
+      <c r="CA1" s="46"/>
+      <c r="CB1" s="46"/>
       <c r="CC1" s="1"/>
-      <c r="CD1" s="84" t="s">
+      <c r="CD1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="CE1" s="84"/>
-      <c r="CF1" s="84"/>
-      <c r="CG1" s="84"/>
-      <c r="CH1" s="84"/>
-      <c r="CI1" s="84"/>
-      <c r="CJ1" s="84"/>
-      <c r="CK1" s="84"/>
-      <c r="CL1" s="84"/>
-      <c r="CM1" s="84"/>
-      <c r="CN1" s="84"/>
-      <c r="CO1" s="84"/>
-      <c r="CP1" s="84"/>
-      <c r="CQ1" s="84"/>
-      <c r="CR1" s="84"/>
-      <c r="CS1" s="84"/>
-      <c r="CT1" s="84"/>
-      <c r="CU1" s="84"/>
-      <c r="CV1" s="84"/>
-      <c r="CW1" s="84"/>
-      <c r="CX1" s="84"/>
-      <c r="CY1" s="84"/>
-      <c r="CZ1" s="84"/>
-      <c r="DA1" s="84"/>
-      <c r="DB1" s="84"/>
-      <c r="DC1" s="84"/>
-      <c r="DD1" s="84"/>
-      <c r="DE1" s="84"/>
-      <c r="DF1" s="84"/>
-      <c r="DG1" s="84"/>
-      <c r="DH1" s="84"/>
-      <c r="DI1" s="84"/>
-      <c r="DJ1" s="84"/>
-      <c r="DK1" s="84"/>
-      <c r="DL1" s="84"/>
-      <c r="DM1" s="84"/>
-      <c r="DN1" s="84"/>
-      <c r="DO1" s="84"/>
-      <c r="DP1" s="84"/>
+      <c r="CE1" s="47"/>
+      <c r="CF1" s="47"/>
+      <c r="CG1" s="47"/>
+      <c r="CH1" s="47"/>
+      <c r="CI1" s="47"/>
+      <c r="CJ1" s="47"/>
+      <c r="CK1" s="47"/>
+      <c r="CL1" s="47"/>
+      <c r="CM1" s="47"/>
+      <c r="CN1" s="47"/>
+      <c r="CO1" s="47"/>
+      <c r="CP1" s="47"/>
+      <c r="CQ1" s="47"/>
+      <c r="CR1" s="47"/>
+      <c r="CS1" s="47"/>
+      <c r="CT1" s="47"/>
+      <c r="CU1" s="47"/>
+      <c r="CV1" s="47"/>
+      <c r="CW1" s="47"/>
+      <c r="CX1" s="47"/>
+      <c r="CY1" s="47"/>
+      <c r="CZ1" s="47"/>
+      <c r="DA1" s="47"/>
+      <c r="DB1" s="47"/>
+      <c r="DC1" s="47"/>
+      <c r="DD1" s="47"/>
+      <c r="DE1" s="47"/>
+      <c r="DF1" s="47"/>
+      <c r="DG1" s="47"/>
+      <c r="DH1" s="47"/>
+      <c r="DI1" s="47"/>
+      <c r="DJ1" s="47"/>
+      <c r="DK1" s="47"/>
+      <c r="DL1" s="47"/>
+      <c r="DM1" s="47"/>
+      <c r="DN1" s="47"/>
+      <c r="DO1" s="47"/>
+      <c r="DP1" s="47"/>
       <c r="DQ1" s="1"/>
-      <c r="DR1" s="85" t="s">
+      <c r="DR1" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="DS1" s="85"/>
-      <c r="DT1" s="85"/>
-      <c r="DU1" s="85"/>
-      <c r="DV1" s="85"/>
-      <c r="DW1" s="85"/>
-      <c r="DX1" s="85"/>
-      <c r="DY1" s="85"/>
-      <c r="DZ1" s="85"/>
-      <c r="EA1" s="85"/>
-      <c r="EB1" s="85"/>
-      <c r="EC1" s="85"/>
-      <c r="ED1" s="85"/>
-      <c r="EE1" s="85"/>
-      <c r="EF1" s="85"/>
+      <c r="DS1" s="48"/>
+      <c r="DT1" s="48"/>
+      <c r="DU1" s="48"/>
+      <c r="DV1" s="48"/>
+      <c r="DW1" s="48"/>
+      <c r="DX1" s="48"/>
+      <c r="DY1" s="48"/>
+      <c r="DZ1" s="48"/>
+      <c r="EA1" s="48"/>
+      <c r="EB1" s="48"/>
+      <c r="EC1" s="48"/>
+      <c r="ED1" s="48"/>
+      <c r="EE1" s="48"/>
+      <c r="EF1" s="48"/>
       <c r="EG1" s="1"/>
-      <c r="EH1" s="92" t="s">
+      <c r="EH1" s="44" t="s">
         <v>5</v>
       </c>
-      <c r="EI1" s="92"/>
-      <c r="EJ1" s="92"/>
-      <c r="EK1" s="92"/>
-      <c r="EL1" s="92"/>
-      <c r="EM1" s="92"/>
-      <c r="EN1" s="92"/>
-      <c r="EO1" s="92"/>
-      <c r="EP1" s="92"/>
-      <c r="EQ1" s="92"/>
-      <c r="ER1" s="92"/>
-      <c r="ES1" s="92"/>
-      <c r="ET1" s="92"/>
-      <c r="EU1" s="92"/>
-      <c r="EV1" s="92"/>
+      <c r="EI1" s="44"/>
+      <c r="EJ1" s="44"/>
+      <c r="EK1" s="44"/>
+      <c r="EL1" s="44"/>
+      <c r="EM1" s="44"/>
+      <c r="EN1" s="44"/>
+      <c r="EO1" s="44"/>
+      <c r="EP1" s="44"/>
+      <c r="EQ1" s="44"/>
+      <c r="ER1" s="44"/>
+      <c r="ES1" s="44"/>
+      <c r="ET1" s="44"/>
+      <c r="EU1" s="44"/>
+      <c r="EV1" s="44"/>
       <c r="EW1" s="1"/>
-      <c r="EX1" s="90" t="s">
+      <c r="EX1" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="EY1" s="90"/>
-      <c r="EZ1" s="90"/>
-      <c r="FA1" s="90"/>
-      <c r="FB1" s="90"/>
-      <c r="FC1" s="90"/>
-      <c r="FD1" s="90"/>
+      <c r="EY1" s="43"/>
+      <c r="EZ1" s="43"/>
+      <c r="FA1" s="43"/>
+      <c r="FB1" s="43"/>
+      <c r="FC1" s="43"/>
+      <c r="FD1" s="43"/>
       <c r="FE1" s="1"/>
-      <c r="FF1" s="93" t="s">
+      <c r="FF1" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="FG1" s="93"/>
-      <c r="FH1" s="93"/>
-      <c r="FI1" s="93"/>
-      <c r="FJ1" s="93"/>
-      <c r="FK1" s="93"/>
-      <c r="FL1" s="93"/>
+      <c r="FG1" s="38"/>
+      <c r="FH1" s="38"/>
+      <c r="FI1" s="38"/>
+      <c r="FJ1" s="38"/>
+      <c r="FK1" s="38"/>
+      <c r="FL1" s="38"/>
       <c r="FM1" s="1"/>
-      <c r="FN1" s="94" t="s">
+      <c r="FN1" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="FO1" s="94"/>
-      <c r="FP1" s="94"/>
-      <c r="FQ1" s="94"/>
-      <c r="FR1" s="94"/>
-      <c r="FS1" s="94"/>
-      <c r="FT1" s="94"/>
+      <c r="FO1" s="40"/>
+      <c r="FP1" s="40"/>
+      <c r="FQ1" s="40"/>
+      <c r="FR1" s="40"/>
+      <c r="FS1" s="40"/>
+      <c r="FT1" s="40"/>
       <c r="FU1" s="1"/>
     </row>
     <row r="2" spans="1:177" x14ac:dyDescent="0.2">
-      <c r="A2" s="82"/>
-      <c r="B2" s="91" t="s">
+      <c r="A2" s="45"/>
+      <c r="B2" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="91"/>
-      <c r="D2" s="91"/>
-      <c r="E2" s="91"/>
-      <c r="F2" s="91"/>
-      <c r="G2" s="91"/>
-      <c r="H2" s="91"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
       <c r="I2" s="1"/>
-      <c r="J2" s="86" t="s">
+      <c r="J2" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="86"/>
-      <c r="L2" s="86"/>
-      <c r="M2" s="86"/>
-      <c r="N2" s="86"/>
-      <c r="O2" s="86"/>
-      <c r="P2" s="86"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="39"/>
       <c r="Q2" s="1"/>
-      <c r="R2" s="86" t="s">
+      <c r="R2" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="S2" s="86"/>
-      <c r="T2" s="86"/>
-      <c r="U2" s="86"/>
-      <c r="V2" s="86"/>
-      <c r="W2" s="86"/>
-      <c r="X2" s="86"/>
+      <c r="S2" s="39"/>
+      <c r="T2" s="39"/>
+      <c r="U2" s="39"/>
+      <c r="V2" s="39"/>
+      <c r="W2" s="39"/>
+      <c r="X2" s="39"/>
       <c r="Y2" s="1"/>
-      <c r="Z2" s="86" t="s">
+      <c r="Z2" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="AA2" s="86"/>
-      <c r="AB2" s="86"/>
-      <c r="AC2" s="86"/>
-      <c r="AD2" s="86"/>
-      <c r="AE2" s="86"/>
-      <c r="AF2" s="86"/>
+      <c r="AA2" s="39"/>
+      <c r="AB2" s="39"/>
+      <c r="AC2" s="39"/>
+      <c r="AD2" s="39"/>
+      <c r="AE2" s="39"/>
+      <c r="AF2" s="39"/>
       <c r="AG2" s="1"/>
-      <c r="AH2" s="86" t="s">
+      <c r="AH2" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="AI2" s="86"/>
-      <c r="AJ2" s="86"/>
-      <c r="AK2" s="86"/>
-      <c r="AL2" s="86"/>
-      <c r="AM2" s="86"/>
-      <c r="AN2" s="86"/>
+      <c r="AI2" s="39"/>
+      <c r="AJ2" s="39"/>
+      <c r="AK2" s="39"/>
+      <c r="AL2" s="39"/>
+      <c r="AM2" s="39"/>
+      <c r="AN2" s="39"/>
       <c r="AO2" s="1"/>
-      <c r="AP2" s="86" t="s">
+      <c r="AP2" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="AQ2" s="86"/>
-      <c r="AR2" s="86"/>
-      <c r="AS2" s="86"/>
-      <c r="AT2" s="86"/>
-      <c r="AU2" s="86"/>
-      <c r="AV2" s="86"/>
+      <c r="AQ2" s="39"/>
+      <c r="AR2" s="39"/>
+      <c r="AS2" s="39"/>
+      <c r="AT2" s="39"/>
+      <c r="AU2" s="39"/>
+      <c r="AV2" s="39"/>
       <c r="AW2" s="1"/>
-      <c r="AX2" s="88" t="s">
+      <c r="AX2" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="AY2" s="88"/>
-      <c r="AZ2" s="88"/>
-      <c r="BA2" s="88"/>
-      <c r="BB2" s="88"/>
-      <c r="BC2" s="88"/>
-      <c r="BD2" s="89"/>
+      <c r="AY2" s="49"/>
+      <c r="AZ2" s="49"/>
+      <c r="BA2" s="49"/>
+      <c r="BB2" s="49"/>
+      <c r="BC2" s="49"/>
+      <c r="BD2" s="50"/>
       <c r="BE2" s="1"/>
-      <c r="BF2" s="88" t="s">
+      <c r="BF2" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="BG2" s="88"/>
-      <c r="BH2" s="88"/>
-      <c r="BI2" s="88"/>
-      <c r="BJ2" s="88"/>
-      <c r="BK2" s="89"/>
+      <c r="BG2" s="49"/>
+      <c r="BH2" s="49"/>
+      <c r="BI2" s="49"/>
+      <c r="BJ2" s="49"/>
+      <c r="BK2" s="50"/>
       <c r="BL2" s="2"/>
       <c r="BM2" s="1"/>
-      <c r="BN2" s="86" t="s">
+      <c r="BN2" s="39" t="s">
         <v>17</v>
       </c>
-      <c r="BO2" s="86"/>
-      <c r="BP2" s="86"/>
-      <c r="BQ2" s="86"/>
-      <c r="BR2" s="86"/>
-      <c r="BS2" s="86"/>
-      <c r="BT2" s="86"/>
+      <c r="BO2" s="39"/>
+      <c r="BP2" s="39"/>
+      <c r="BQ2" s="39"/>
+      <c r="BR2" s="39"/>
+      <c r="BS2" s="39"/>
+      <c r="BT2" s="39"/>
       <c r="BU2" s="1"/>
-      <c r="BV2" s="86" t="s">
+      <c r="BV2" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="BW2" s="86"/>
-      <c r="BX2" s="86"/>
-      <c r="BY2" s="86"/>
-      <c r="BZ2" s="86"/>
-      <c r="CA2" s="86"/>
-      <c r="CB2" s="86"/>
+      <c r="BW2" s="39"/>
+      <c r="BX2" s="39"/>
+      <c r="BY2" s="39"/>
+      <c r="BZ2" s="39"/>
+      <c r="CA2" s="39"/>
+      <c r="CB2" s="39"/>
       <c r="CC2" s="1"/>
-      <c r="CD2" s="86" t="s">
+      <c r="CD2" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="CE2" s="86"/>
-      <c r="CF2" s="86"/>
-      <c r="CG2" s="86"/>
-      <c r="CH2" s="86"/>
-      <c r="CI2" s="86"/>
-      <c r="CJ2" s="86"/>
+      <c r="CE2" s="39"/>
+      <c r="CF2" s="39"/>
+      <c r="CG2" s="39"/>
+      <c r="CH2" s="39"/>
+      <c r="CI2" s="39"/>
+      <c r="CJ2" s="39"/>
       <c r="CK2" s="1"/>
-      <c r="CL2" s="86" t="s">
+      <c r="CL2" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="CM2" s="86"/>
-      <c r="CN2" s="86"/>
-      <c r="CO2" s="86"/>
-      <c r="CP2" s="86"/>
-      <c r="CQ2" s="86"/>
-      <c r="CR2" s="86"/>
+      <c r="CM2" s="39"/>
+      <c r="CN2" s="39"/>
+      <c r="CO2" s="39"/>
+      <c r="CP2" s="39"/>
+      <c r="CQ2" s="39"/>
+      <c r="CR2" s="39"/>
       <c r="CS2" s="1"/>
-      <c r="CT2" s="86" t="s">
+      <c r="CT2" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="CU2" s="86"/>
-      <c r="CV2" s="86"/>
-      <c r="CW2" s="86"/>
-      <c r="CX2" s="86"/>
-      <c r="CY2" s="86"/>
-      <c r="CZ2" s="86"/>
+      <c r="CU2" s="39"/>
+      <c r="CV2" s="39"/>
+      <c r="CW2" s="39"/>
+      <c r="CX2" s="39"/>
+      <c r="CY2" s="39"/>
+      <c r="CZ2" s="39"/>
       <c r="DA2" s="1"/>
-      <c r="DB2" s="86" t="s">
+      <c r="DB2" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="DC2" s="86"/>
-      <c r="DD2" s="86"/>
-      <c r="DE2" s="86"/>
-      <c r="DF2" s="86"/>
-      <c r="DG2" s="86"/>
-      <c r="DH2" s="86"/>
+      <c r="DC2" s="39"/>
+      <c r="DD2" s="39"/>
+      <c r="DE2" s="39"/>
+      <c r="DF2" s="39"/>
+      <c r="DG2" s="39"/>
+      <c r="DH2" s="39"/>
       <c r="DI2" s="1"/>
-      <c r="DJ2" s="86" t="s">
+      <c r="DJ2" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="DK2" s="86"/>
-      <c r="DL2" s="86"/>
-      <c r="DM2" s="86"/>
-      <c r="DN2" s="86"/>
-      <c r="DO2" s="86"/>
-      <c r="DP2" s="86"/>
+      <c r="DK2" s="39"/>
+      <c r="DL2" s="39"/>
+      <c r="DM2" s="39"/>
+      <c r="DN2" s="39"/>
+      <c r="DO2" s="39"/>
+      <c r="DP2" s="39"/>
       <c r="DQ2" s="1"/>
-      <c r="DR2" s="86" t="s">
+      <c r="DR2" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="DS2" s="86"/>
-      <c r="DT2" s="86"/>
-      <c r="DU2" s="86"/>
-      <c r="DV2" s="86"/>
-      <c r="DW2" s="86"/>
-      <c r="DX2" s="86"/>
+      <c r="DS2" s="39"/>
+      <c r="DT2" s="39"/>
+      <c r="DU2" s="39"/>
+      <c r="DV2" s="39"/>
+      <c r="DW2" s="39"/>
+      <c r="DX2" s="39"/>
       <c r="DY2" s="1"/>
-      <c r="DZ2" s="86" t="s">
+      <c r="DZ2" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="EA2" s="86"/>
-      <c r="EB2" s="86"/>
-      <c r="EC2" s="86"/>
-      <c r="ED2" s="86"/>
-      <c r="EE2" s="86"/>
-      <c r="EF2" s="86"/>
+      <c r="EA2" s="39"/>
+      <c r="EB2" s="39"/>
+      <c r="EC2" s="39"/>
+      <c r="ED2" s="39"/>
+      <c r="EE2" s="39"/>
+      <c r="EF2" s="39"/>
       <c r="EG2" s="1"/>
-      <c r="EH2" s="86" t="s">
+      <c r="EH2" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="EI2" s="86"/>
-      <c r="EJ2" s="86"/>
-      <c r="EK2" s="86"/>
-      <c r="EL2" s="86"/>
-      <c r="EM2" s="86"/>
-      <c r="EN2" s="86"/>
+      <c r="EI2" s="39"/>
+      <c r="EJ2" s="39"/>
+      <c r="EK2" s="39"/>
+      <c r="EL2" s="39"/>
+      <c r="EM2" s="39"/>
+      <c r="EN2" s="39"/>
       <c r="EO2" s="1"/>
-      <c r="EP2" s="86" t="s">
+      <c r="EP2" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="EQ2" s="86"/>
-      <c r="ER2" s="86"/>
-      <c r="ES2" s="86"/>
-      <c r="ET2" s="86"/>
-      <c r="EU2" s="86"/>
-      <c r="EV2" s="86"/>
+      <c r="EQ2" s="39"/>
+      <c r="ER2" s="39"/>
+      <c r="ES2" s="39"/>
+      <c r="ET2" s="39"/>
+      <c r="EU2" s="39"/>
+      <c r="EV2" s="39"/>
       <c r="EW2" s="1"/>
-      <c r="EX2" s="86" t="s">
+      <c r="EX2" s="39" t="s">
         <v>28</v>
       </c>
-      <c r="EY2" s="86"/>
-      <c r="EZ2" s="86"/>
-      <c r="FA2" s="86"/>
-      <c r="FB2" s="86"/>
-      <c r="FC2" s="86"/>
-      <c r="FD2" s="86"/>
+      <c r="EY2" s="39"/>
+      <c r="EZ2" s="39"/>
+      <c r="FA2" s="39"/>
+      <c r="FB2" s="39"/>
+      <c r="FC2" s="39"/>
+      <c r="FD2" s="39"/>
       <c r="FE2" s="1"/>
-      <c r="FF2" s="86" t="s">
+      <c r="FF2" s="39" t="s">
         <v>29</v>
       </c>
-      <c r="FG2" s="86"/>
-      <c r="FH2" s="86"/>
-      <c r="FI2" s="86"/>
-      <c r="FJ2" s="86"/>
-      <c r="FK2" s="86"/>
-      <c r="FL2" s="86"/>
+      <c r="FG2" s="39"/>
+      <c r="FH2" s="39"/>
+      <c r="FI2" s="39"/>
+      <c r="FJ2" s="39"/>
+      <c r="FK2" s="39"/>
+      <c r="FL2" s="39"/>
       <c r="FM2" s="1"/>
-      <c r="FN2" s="86" t="s">
+      <c r="FN2" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="FO2" s="86"/>
-      <c r="FP2" s="86"/>
-      <c r="FQ2" s="86"/>
-      <c r="FR2" s="86"/>
-      <c r="FS2" s="86"/>
-      <c r="FT2" s="86"/>
+      <c r="FO2" s="39"/>
+      <c r="FP2" s="39"/>
+      <c r="FQ2" s="39"/>
+      <c r="FR2" s="39"/>
+      <c r="FS2" s="39"/>
+      <c r="FT2" s="39"/>
       <c r="FU2" s="1"/>
     </row>
     <row r="3" spans="1:177" x14ac:dyDescent="0.2">
-      <c r="A3" s="82"/>
+      <c r="A3" s="45"/>
       <c r="B3" s="11" t="s">
         <v>32</v>
       </c>
@@ -8799,10 +8762,10 @@
       <c r="F18" s="6">
         <v>27463600</v>
       </c>
-      <c r="G18" s="38">
+      <c r="G18" s="10">
         <v>0.151466850667793</v>
       </c>
-      <c r="H18" s="39">
+      <c r="H18" s="10">
         <v>-6.6518847006651251E-3</v>
       </c>
       <c r="I18" s="1"/>
@@ -8821,10 +8784,10 @@
       <c r="N18" s="6">
         <v>23475502</v>
       </c>
-      <c r="O18" s="40">
+      <c r="O18" s="10">
         <v>0.13557426801778297</v>
       </c>
-      <c r="P18" s="41">
+      <c r="P18" s="10">
         <v>-1.0510510510510555E-2</v>
       </c>
       <c r="Q18" s="1"/>
@@ -8843,10 +8806,10 @@
       <c r="V18" s="6">
         <v>2339861</v>
       </c>
-      <c r="W18" s="42">
+      <c r="W18" s="10">
         <v>0.55306105790044791</v>
       </c>
-      <c r="X18" s="43">
+      <c r="X18" s="10">
         <v>-7.0257611241217131E-3</v>
       </c>
       <c r="Y18" s="1"/>
@@ -8865,10 +8828,10 @@
       <c r="AD18" s="6">
         <v>17250007</v>
       </c>
-      <c r="AE18" s="44">
+      <c r="AE18" s="10">
         <v>0.37768042644852262</v>
       </c>
-      <c r="AF18" s="45">
+      <c r="AF18" s="10">
         <v>-1.8276762402088847E-2</v>
       </c>
       <c r="AG18" s="1"/>
@@ -8887,10 +8850,10 @@
       <c r="AL18" s="6">
         <v>13499600</v>
       </c>
-      <c r="AM18" s="46">
+      <c r="AM18" s="10">
         <v>0.11481080920916176</v>
       </c>
-      <c r="AN18" s="47">
+      <c r="AN18" s="10">
         <v>-1.258992805755388E-2</v>
       </c>
       <c r="AO18" s="1"/>
@@ -8909,10 +8872,10 @@
       <c r="AT18" s="6">
         <v>22656100</v>
       </c>
-      <c r="AU18" s="48">
+      <c r="AU18" s="10">
         <v>0.35805632920052438</v>
       </c>
-      <c r="AV18" s="49">
+      <c r="AV18" s="10">
         <v>-9.1743119266055051E-3</v>
       </c>
       <c r="AW18" s="1"/>
@@ -8931,10 +8894,10 @@
       <c r="BB18" s="6">
         <v>10469500</v>
       </c>
-      <c r="BC18" s="50">
+      <c r="BC18" s="10">
         <v>2.5340274129614596E-2</v>
       </c>
-      <c r="BD18" s="51">
+      <c r="BD18" s="10">
         <v>-1.6985138004246225E-2</v>
       </c>
       <c r="BE18" s="1"/>
@@ -8953,10 +8916,10 @@
       <c r="BJ18" s="6">
         <v>7196600</v>
       </c>
-      <c r="BK18" s="52">
+      <c r="BK18" s="10">
         <v>0.18808576272128505</v>
       </c>
-      <c r="BL18" s="53">
+      <c r="BL18" s="10">
         <v>1.2515644555693905E-3</v>
       </c>
       <c r="BM18" s="1"/>
@@ -8975,10 +8938,10 @@
       <c r="BR18" s="6">
         <v>3961100</v>
       </c>
-      <c r="BS18" s="54">
+      <c r="BS18" s="10">
         <v>0.99726212415743098</v>
       </c>
-      <c r="BT18" s="55">
+      <c r="BT18" s="10">
         <v>-6.5645514223194121E-3</v>
       </c>
       <c r="BU18" s="1"/>
@@ -8997,10 +8960,10 @@
       <c r="BZ18" s="6">
         <v>414200</v>
       </c>
-      <c r="CA18" s="56">
+      <c r="CA18" s="10">
         <v>0.83728150651859001</v>
       </c>
-      <c r="CB18" s="57">
+      <c r="CB18" s="10">
         <v>-2.161100196463657E-2</v>
       </c>
       <c r="CC18" s="1"/>
@@ -9019,10 +8982,10 @@
       <c r="CH18" s="6">
         <v>10227900</v>
       </c>
-      <c r="CI18" s="58">
+      <c r="CI18" s="10">
         <v>0.8674600846703624</v>
       </c>
-      <c r="CJ18" s="59">
+      <c r="CJ18" s="10">
         <v>-2.4691358024691357E-2</v>
       </c>
       <c r="CK18" s="1"/>
@@ -9041,10 +9004,10 @@
       <c r="CP18" s="6">
         <v>35007200</v>
       </c>
-      <c r="CQ18" s="60">
+      <c r="CQ18" s="10">
         <v>0.11844717658081766</v>
       </c>
-      <c r="CR18" s="61">
+      <c r="CR18" s="10">
         <v>2.179176755447956E-2</v>
       </c>
       <c r="CS18" s="1"/>
@@ -9063,10 +9026,10 @@
       <c r="CX18" s="6">
         <v>10358600</v>
       </c>
-      <c r="CY18" s="62">
+      <c r="CY18" s="10">
         <v>3.7793041530708782E-2</v>
       </c>
-      <c r="CZ18" s="63">
+      <c r="CZ18" s="10">
         <v>-1.6100178890876539E-2</v>
       </c>
       <c r="DA18" s="1"/>
@@ -9085,10 +9048,10 @@
       <c r="DF18" s="6">
         <v>39037500</v>
       </c>
-      <c r="DG18" s="64">
+      <c r="DG18" s="10">
         <v>2.9750393852065321E-2</v>
       </c>
-      <c r="DH18" s="65">
+      <c r="DH18" s="10">
         <v>-1.098901098901095E-2</v>
       </c>
       <c r="DI18" s="1"/>
@@ -9107,10 +9070,10 @@
       <c r="DN18" s="6">
         <v>5979300</v>
       </c>
-      <c r="DO18" s="66">
+      <c r="DO18" s="10">
         <v>0.15346277992407137</v>
       </c>
-      <c r="DP18" s="67">
+      <c r="DP18" s="10">
         <v>0</v>
       </c>
       <c r="DQ18" s="1"/>
@@ -9129,10 +9092,10 @@
       <c r="DV18" s="6">
         <v>948300</v>
       </c>
-      <c r="DW18" s="68">
+      <c r="DW18" s="10">
         <v>0.23020141305494041</v>
       </c>
-      <c r="DX18" s="69">
+      <c r="DX18" s="10">
         <v>-1.1396011396011355E-2</v>
       </c>
       <c r="DY18" s="1"/>
@@ -9151,10 +9114,10 @@
       <c r="ED18" s="6">
         <v>3180500</v>
       </c>
-      <c r="EE18" s="70">
+      <c r="EE18" s="10">
         <v>3.895613897185977E-3</v>
       </c>
-      <c r="EF18" s="71">
+      <c r="EF18" s="10">
         <v>-1.2178619756427488E-2</v>
       </c>
       <c r="EG18" s="1"/>
@@ -9173,10 +9136,10 @@
       <c r="EL18" s="6">
         <v>1137000</v>
       </c>
-      <c r="EM18" s="72">
+      <c r="EM18" s="10">
         <v>4.283201407211961E-2</v>
       </c>
-      <c r="EN18" s="73">
+      <c r="EN18" s="10">
         <v>-1.7080745341614818E-2</v>
       </c>
       <c r="EO18" s="1"/>
@@ -9195,10 +9158,10 @@
       <c r="ET18" s="6">
         <v>11721200</v>
       </c>
-      <c r="EU18" s="74">
+      <c r="EU18" s="10">
         <v>2.9706855953315361E-2</v>
       </c>
-      <c r="EV18" s="75">
+      <c r="EV18" s="10">
         <v>4.0983606557377632E-3</v>
       </c>
       <c r="EW18" s="1"/>
@@ -9217,10 +9180,10 @@
       <c r="FB18" s="6">
         <v>28094000</v>
       </c>
-      <c r="FC18" s="76">
+      <c r="FC18" s="10">
         <v>1.9250409340072612E-2</v>
       </c>
-      <c r="FD18" s="77">
+      <c r="FD18" s="10">
         <v>6.410256410256502E-3</v>
       </c>
       <c r="FE18" s="1"/>
@@ -9239,10 +9202,10 @@
       <c r="FJ18" s="6">
         <v>2049000</v>
       </c>
-      <c r="FK18" s="78">
+      <c r="FK18" s="10">
         <v>7.2027818448023431E-2</v>
       </c>
-      <c r="FL18" s="79">
+      <c r="FL18" s="10">
         <v>-4.1109969167523706E-3</v>
       </c>
       <c r="FM18" s="1"/>
@@ -9261,10 +9224,10 @@
       <c r="FR18" s="6">
         <v>1425500</v>
       </c>
-      <c r="FS18" s="80">
+      <c r="FS18" s="10">
         <v>0.28172571027709575</v>
       </c>
-      <c r="FT18" s="81">
+      <c r="FT18" s="10">
         <v>3.0478955007256808E-2</v>
       </c>
       <c r="FU18" s="1"/>
@@ -9273,181 +9236,489 @@
       <c r="A19" s="5">
         <v>45266</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="35"/>
+      <c r="B19" s="6">
+        <v>844395</v>
+      </c>
+      <c r="C19" s="6">
+        <v>4611723</v>
+      </c>
+      <c r="D19" s="6">
+        <v>-3767328</v>
+      </c>
+      <c r="E19" s="6">
+        <v>-85564760000</v>
+      </c>
+      <c r="F19" s="6">
+        <v>30761300</v>
+      </c>
+      <c r="G19" s="10">
+        <v>0.17736955200202853</v>
+      </c>
+      <c r="H19" s="10">
+        <v>8.8691796008868867E-3</v>
+      </c>
       <c r="I19" s="1"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="6"/>
-      <c r="M19" s="6"/>
-      <c r="N19" s="6"/>
-      <c r="O19" s="34"/>
-      <c r="P19" s="35"/>
+      <c r="J19" s="6">
+        <v>4023800</v>
+      </c>
+      <c r="K19" s="6">
+        <v>3214745</v>
+      </c>
+      <c r="L19" s="6">
+        <v>809055</v>
+      </c>
+      <c r="M19" s="6">
+        <v>27324430000</v>
+      </c>
+      <c r="N19" s="6">
+        <v>17934800</v>
+      </c>
+      <c r="O19" s="10">
+        <v>0.40360332983919534</v>
+      </c>
+      <c r="P19" s="10">
+        <v>7.4962518740629685E-3</v>
+      </c>
       <c r="Q19" s="1"/>
-      <c r="R19" s="6"/>
-      <c r="S19" s="6"/>
-      <c r="T19" s="6"/>
-      <c r="U19" s="6"/>
-      <c r="V19" s="6"/>
-      <c r="W19" s="34"/>
-      <c r="X19" s="35"/>
+      <c r="R19" s="6">
+        <v>200511</v>
+      </c>
+      <c r="S19" s="6">
+        <v>189983</v>
+      </c>
+      <c r="T19" s="6">
+        <v>10528</v>
+      </c>
+      <c r="U19" s="6">
+        <v>925310000</v>
+      </c>
+      <c r="V19" s="6">
+        <v>748000</v>
+      </c>
+      <c r="W19" s="10">
+        <v>0.52205080213903743</v>
+      </c>
+      <c r="X19" s="10">
+        <v>7.033997655334215E-3</v>
+      </c>
       <c r="Y19" s="1"/>
-      <c r="Z19" s="6"/>
-      <c r="AA19" s="6"/>
-      <c r="AB19" s="6"/>
-      <c r="AC19" s="6"/>
-      <c r="AD19" s="6"/>
-      <c r="AE19" s="34"/>
-      <c r="AF19" s="35"/>
+      <c r="Z19" s="6">
+        <v>2982043</v>
+      </c>
+      <c r="AA19" s="6">
+        <v>4331520</v>
+      </c>
+      <c r="AB19" s="6">
+        <v>-1349477</v>
+      </c>
+      <c r="AC19" s="6">
+        <v>-26079720000</v>
+      </c>
+      <c r="AD19" s="6">
+        <v>13820007</v>
+      </c>
+      <c r="AE19" s="10">
+        <v>0.52920110677223242</v>
+      </c>
+      <c r="AF19" s="10">
+        <v>7.7922077922077185E-3</v>
+      </c>
       <c r="AG19" s="1"/>
-      <c r="AH19" s="6"/>
-      <c r="AI19" s="6"/>
-      <c r="AJ19" s="6"/>
-      <c r="AK19" s="6"/>
-      <c r="AL19" s="6"/>
-      <c r="AM19" s="34"/>
-      <c r="AN19" s="35"/>
+      <c r="AH19" s="6">
+        <v>709100</v>
+      </c>
+      <c r="AI19" s="6">
+        <v>2349700</v>
+      </c>
+      <c r="AJ19" s="6">
+        <v>-1640600</v>
+      </c>
+      <c r="AK19" s="6">
+        <v>-45769150000</v>
+      </c>
+      <c r="AL19" s="6">
+        <v>14176100</v>
+      </c>
+      <c r="AM19" s="10">
+        <v>0.21577161560654906</v>
+      </c>
+      <c r="AN19" s="10">
+        <v>1.4440433212996467E-2</v>
+      </c>
       <c r="AO19" s="1"/>
-      <c r="AP19" s="6"/>
-      <c r="AQ19" s="6"/>
-      <c r="AR19" s="6"/>
-      <c r="AS19" s="6"/>
-      <c r="AT19" s="6"/>
-      <c r="AU19" s="34"/>
-      <c r="AV19" s="35"/>
+      <c r="AP19" s="6">
+        <v>1578400</v>
+      </c>
+      <c r="AQ19" s="6">
+        <v>662601</v>
+      </c>
+      <c r="AR19" s="6">
+        <v>915799</v>
+      </c>
+      <c r="AS19" s="6">
+        <v>25160410000</v>
+      </c>
+      <c r="AT19" s="6">
+        <v>18648100</v>
+      </c>
+      <c r="AU19" s="10">
+        <v>0.12017315436961407</v>
+      </c>
+      <c r="AV19" s="10">
+        <v>1.2844036697247759E-2</v>
+      </c>
       <c r="AW19" s="1"/>
-      <c r="AX19" s="6"/>
-      <c r="AY19" s="6"/>
-      <c r="AZ19" s="6"/>
-      <c r="BA19" s="6"/>
-      <c r="BB19" s="6"/>
-      <c r="BC19" s="34"/>
-      <c r="BD19" s="35"/>
+      <c r="AX19" s="6">
+        <v>314700</v>
+      </c>
+      <c r="AY19" s="6">
+        <v>657900</v>
+      </c>
+      <c r="AZ19" s="6">
+        <v>-343200</v>
+      </c>
+      <c r="BA19" s="6">
+        <v>-8007690000</v>
+      </c>
+      <c r="BB19" s="6">
+        <v>12297500</v>
+      </c>
+      <c r="BC19" s="10">
+        <v>7.9089245781662945E-2</v>
+      </c>
+      <c r="BD19" s="10">
+        <v>8.5106382978723093E-3</v>
+      </c>
       <c r="BE19" s="1"/>
-      <c r="BF19" s="6"/>
-      <c r="BG19" s="6"/>
-      <c r="BH19" s="6"/>
-      <c r="BI19" s="6"/>
-      <c r="BJ19" s="6"/>
-      <c r="BK19" s="34"/>
-      <c r="BL19" s="35"/>
+      <c r="BF19" s="6">
+        <v>1148400</v>
+      </c>
+      <c r="BG19" s="6">
+        <v>1514000</v>
+      </c>
+      <c r="BH19" s="6">
+        <v>-365600</v>
+      </c>
+      <c r="BI19" s="6">
+        <v>-14764250000</v>
+      </c>
+      <c r="BJ19" s="6">
+        <v>9776800</v>
+      </c>
+      <c r="BK19" s="10">
+        <v>0.27231814090499962</v>
+      </c>
+      <c r="BL19" s="10">
+        <v>2.375000000000007E-2</v>
+      </c>
       <c r="BM19" s="1"/>
-      <c r="BN19" s="6"/>
-      <c r="BO19" s="6"/>
-      <c r="BP19" s="6"/>
-      <c r="BQ19" s="6"/>
-      <c r="BR19" s="6"/>
-      <c r="BS19" s="34"/>
-      <c r="BT19" s="35"/>
+      <c r="BN19" s="6">
+        <v>609200</v>
+      </c>
+      <c r="BO19" s="6">
+        <v>1668700</v>
+      </c>
+      <c r="BP19" s="6">
+        <v>-1059500</v>
+      </c>
+      <c r="BQ19" s="6">
+        <v>-24176450000</v>
+      </c>
+      <c r="BR19" s="6">
+        <v>3749700</v>
+      </c>
+      <c r="BS19" s="10">
+        <v>0.60748859908792707</v>
+      </c>
+      <c r="BT19" s="10">
+        <v>2.1881838074397004E-3</v>
+      </c>
       <c r="BU19" s="1"/>
-      <c r="BV19" s="6"/>
-      <c r="BW19" s="6"/>
-      <c r="BX19" s="6"/>
-      <c r="BY19" s="6"/>
-      <c r="BZ19" s="6"/>
-      <c r="CA19" s="34"/>
-      <c r="CB19" s="35"/>
+      <c r="BV19" s="6">
+        <v>44600</v>
+      </c>
+      <c r="BW19" s="6">
+        <v>191572</v>
+      </c>
+      <c r="BX19" s="6">
+        <v>-146972</v>
+      </c>
+      <c r="BY19" s="6">
+        <v>-14702700000</v>
+      </c>
+      <c r="BZ19" s="6">
+        <v>553800</v>
+      </c>
+      <c r="CA19" s="10">
+        <v>0.42645720476706395</v>
+      </c>
+      <c r="CB19" s="10">
+        <v>0</v>
+      </c>
       <c r="CC19" s="1"/>
-      <c r="CD19" s="6"/>
-      <c r="CE19" s="6"/>
-      <c r="CF19" s="6"/>
-      <c r="CG19" s="6"/>
-      <c r="CH19" s="6"/>
-      <c r="CI19" s="34"/>
-      <c r="CJ19" s="35"/>
+      <c r="CD19" s="6">
+        <v>752100</v>
+      </c>
+      <c r="CE19" s="6">
+        <v>6852740</v>
+      </c>
+      <c r="CF19" s="6">
+        <v>-6100640</v>
+      </c>
+      <c r="CG19" s="6">
+        <v>-244284260000</v>
+      </c>
+      <c r="CH19" s="6">
+        <v>11848000</v>
+      </c>
+      <c r="CI19" s="10">
+        <v>0.64186698176907497</v>
+      </c>
+      <c r="CJ19" s="10">
+        <v>-1.2360939431396083E-3</v>
+      </c>
       <c r="CK19" s="1"/>
-      <c r="CL19" s="6"/>
-      <c r="CM19" s="6"/>
-      <c r="CN19" s="6"/>
-      <c r="CO19" s="6"/>
-      <c r="CP19" s="6"/>
-      <c r="CQ19" s="34"/>
-      <c r="CR19" s="35"/>
+      <c r="CL19" s="6">
+        <v>193300</v>
+      </c>
+      <c r="CM19" s="6">
+        <v>2100196</v>
+      </c>
+      <c r="CN19" s="6">
+        <v>-1906896</v>
+      </c>
+      <c r="CO19" s="6">
+        <v>-40114500000</v>
+      </c>
+      <c r="CP19" s="6">
+        <v>24909300</v>
+      </c>
+      <c r="CQ19" s="10">
+        <v>9.2073884051338262E-2</v>
+      </c>
+      <c r="CR19" s="10">
+        <v>9.4786729857819566E-3</v>
+      </c>
       <c r="CS19" s="1"/>
-      <c r="CT19" s="6"/>
-      <c r="CU19" s="6"/>
-      <c r="CV19" s="6"/>
-      <c r="CW19" s="6"/>
-      <c r="CX19" s="6"/>
-      <c r="CY19" s="34"/>
-      <c r="CZ19" s="35"/>
+      <c r="CT19" s="6">
+        <v>503951</v>
+      </c>
+      <c r="CU19" s="6">
+        <v>111500</v>
+      </c>
+      <c r="CV19" s="6">
+        <v>392451</v>
+      </c>
+      <c r="CW19" s="6">
+        <v>11126460000</v>
+      </c>
+      <c r="CX19" s="6">
+        <v>16609000</v>
+      </c>
+      <c r="CY19" s="10">
+        <v>3.7055271238485156E-2</v>
+      </c>
+      <c r="CZ19" s="10">
+        <v>2.8571428571428598E-2</v>
+      </c>
       <c r="DA19" s="1"/>
-      <c r="DB19" s="6"/>
-      <c r="DC19" s="6"/>
-      <c r="DD19" s="6"/>
-      <c r="DE19" s="6"/>
-      <c r="DF19" s="6"/>
-      <c r="DG19" s="34"/>
-      <c r="DH19" s="35"/>
+      <c r="DB19" s="6">
+        <v>655303</v>
+      </c>
+      <c r="DC19" s="6">
+        <v>978500</v>
+      </c>
+      <c r="DD19" s="6">
+        <v>-323197</v>
+      </c>
+      <c r="DE19" s="6">
+        <v>-5849600000</v>
+      </c>
+      <c r="DF19" s="6">
+        <v>24850100</v>
+      </c>
+      <c r="DG19" s="10">
+        <v>6.5746335024808755E-2</v>
+      </c>
+      <c r="DH19" s="10">
+        <v>2.7397260273972993E-3</v>
+      </c>
       <c r="DI19" s="1"/>
-      <c r="DJ19" s="6"/>
-      <c r="DK19" s="6"/>
-      <c r="DL19" s="6"/>
-      <c r="DM19" s="6"/>
-      <c r="DN19" s="6"/>
-      <c r="DO19" s="34"/>
-      <c r="DP19" s="35"/>
+      <c r="DJ19" s="6">
+        <v>1293500</v>
+      </c>
+      <c r="DK19" s="6">
+        <v>1767900</v>
+      </c>
+      <c r="DL19" s="6">
+        <v>-474400</v>
+      </c>
+      <c r="DM19" s="6">
+        <v>-15472340000</v>
+      </c>
+      <c r="DN19" s="6">
+        <v>8941800</v>
+      </c>
+      <c r="DO19" s="10">
+        <v>0.3423695452817106</v>
+      </c>
+      <c r="DP19" s="10">
+        <v>-1.5128593040848492E-3</v>
+      </c>
       <c r="DQ19" s="1"/>
-      <c r="DR19" s="6"/>
-      <c r="DS19" s="6"/>
-      <c r="DT19" s="6"/>
-      <c r="DU19" s="6"/>
-      <c r="DV19" s="6"/>
-      <c r="DW19" s="34"/>
-      <c r="DX19" s="35"/>
+      <c r="DR19" s="6">
+        <v>269500</v>
+      </c>
+      <c r="DS19" s="6">
+        <v>220500</v>
+      </c>
+      <c r="DT19" s="6">
+        <v>49000</v>
+      </c>
+      <c r="DU19" s="6">
+        <v>3412710000</v>
+      </c>
+      <c r="DV19" s="6">
+        <v>731000</v>
+      </c>
+      <c r="DW19" s="10">
+        <v>0.6703146374829001</v>
+      </c>
+      <c r="DX19" s="10">
+        <v>1.4204545454544646E-3</v>
+      </c>
       <c r="DY19" s="1"/>
-      <c r="DZ19" s="6"/>
-      <c r="EA19" s="6"/>
-      <c r="EB19" s="6"/>
-      <c r="EC19" s="6"/>
-      <c r="ED19" s="6"/>
-      <c r="EE19" s="34"/>
-      <c r="EF19" s="35"/>
+      <c r="DZ19" s="6">
+        <v>300</v>
+      </c>
+      <c r="EA19" s="6">
+        <v>51800</v>
+      </c>
+      <c r="EB19" s="6">
+        <v>-51500</v>
+      </c>
+      <c r="EC19" s="6">
+        <v>-1939380000</v>
+      </c>
+      <c r="ED19" s="6">
+        <v>2576400</v>
+      </c>
+      <c r="EE19" s="10">
+        <v>2.0222015215028723E-2</v>
+      </c>
+      <c r="EF19" s="10">
+        <v>1.902173913043486E-2</v>
+      </c>
       <c r="EG19" s="1"/>
-      <c r="EH19" s="6"/>
-      <c r="EI19" s="6"/>
-      <c r="EJ19" s="6"/>
-      <c r="EK19" s="6"/>
-      <c r="EL19" s="6"/>
-      <c r="EM19" s="34"/>
-      <c r="EN19" s="35"/>
+      <c r="EH19" s="6">
+        <v>3300</v>
+      </c>
+      <c r="EI19" s="6">
+        <v>100</v>
+      </c>
+      <c r="EJ19" s="6">
+        <v>3200</v>
+      </c>
+      <c r="EK19" s="6">
+        <v>208870000</v>
+      </c>
+      <c r="EL19" s="6">
+        <v>1285400</v>
+      </c>
+      <c r="EM19" s="10">
+        <v>2.6450910222498834E-3</v>
+      </c>
+      <c r="EN19" s="10">
+        <v>2.0186335403726663E-2</v>
+      </c>
       <c r="EO19" s="1"/>
-      <c r="EP19" s="6"/>
-      <c r="EQ19" s="6"/>
-      <c r="ER19" s="6"/>
-      <c r="ES19" s="6"/>
-      <c r="ET19" s="6"/>
-      <c r="EU19" s="34"/>
-      <c r="EV19" s="35"/>
+      <c r="EP19" s="6">
+        <v>313500</v>
+      </c>
+      <c r="EQ19" s="6">
+        <v>55600</v>
+      </c>
+      <c r="ER19" s="6">
+        <v>257900</v>
+      </c>
+      <c r="ES19" s="6">
+        <v>6400680000</v>
+      </c>
+      <c r="ET19" s="6">
+        <v>7038600</v>
+      </c>
+      <c r="EU19" s="10">
+        <v>5.2439405563606399E-2</v>
+      </c>
+      <c r="EV19" s="10">
+        <v>8.1300813008129795E-3</v>
+      </c>
       <c r="EW19" s="1"/>
-      <c r="EX19" s="6"/>
-      <c r="EY19" s="6"/>
-      <c r="EZ19" s="6"/>
-      <c r="FA19" s="6"/>
-      <c r="FB19" s="6"/>
-      <c r="FC19" s="34"/>
-      <c r="FD19" s="35"/>
+      <c r="EX19" s="6">
+        <v>174100</v>
+      </c>
+      <c r="EY19" s="6">
+        <v>301300</v>
+      </c>
+      <c r="EZ19" s="6">
+        <v>-127200</v>
+      </c>
+      <c r="FA19" s="6">
+        <v>-3019530000</v>
+      </c>
+      <c r="FB19" s="6">
+        <v>19894000</v>
+      </c>
+      <c r="FC19" s="10">
+        <v>2.3896652256961897E-2</v>
+      </c>
+      <c r="FD19" s="10">
+        <v>1.2684989429175507E-2</v>
+      </c>
       <c r="FE19" s="1"/>
-      <c r="FF19" s="6"/>
-      <c r="FG19" s="6"/>
-      <c r="FH19" s="6"/>
-      <c r="FI19" s="6"/>
-      <c r="FJ19" s="6"/>
-      <c r="FK19" s="34"/>
-      <c r="FL19" s="35"/>
+      <c r="FF19" s="6">
+        <v>287200</v>
+      </c>
+      <c r="FG19" s="6">
+        <v>36400</v>
+      </c>
+      <c r="FH19" s="6">
+        <v>250800</v>
+      </c>
+      <c r="FI19" s="6">
+        <v>24542520000</v>
+      </c>
+      <c r="FJ19" s="6">
+        <v>1586400</v>
+      </c>
+      <c r="FK19" s="10">
+        <v>0.20398386283408976</v>
+      </c>
+      <c r="FL19" s="10">
+        <v>1.0309278350515464E-2</v>
+      </c>
       <c r="FM19" s="1"/>
-      <c r="FN19" s="6"/>
-      <c r="FO19" s="6"/>
-      <c r="FP19" s="6"/>
-      <c r="FQ19" s="6"/>
-      <c r="FR19" s="6"/>
-      <c r="FS19" s="34"/>
-      <c r="FT19" s="35"/>
+      <c r="FN19" s="6">
+        <v>1666600</v>
+      </c>
+      <c r="FO19" s="6">
+        <v>272700</v>
+      </c>
+      <c r="FP19" s="6">
+        <v>1393900</v>
+      </c>
+      <c r="FQ19" s="6">
+        <v>103324230000</v>
+      </c>
+      <c r="FR19" s="6">
+        <v>2765700</v>
+      </c>
+      <c r="FS19" s="10">
+        <v>0.70119680370249848</v>
+      </c>
+      <c r="FT19" s="10">
+        <v>6.1538461538461618E-2</v>
+      </c>
       <c r="FU19" s="1"/>
     </row>
     <row r="20" spans="1:177" x14ac:dyDescent="0.2">
@@ -11576,117 +11847,117 @@
     </row>
     <row r="32" spans="1:177" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B32" s="6"/>
       <c r="H32" s="10">
         <f>'VNINDEX T11-T12'!D27</f>
-        <v>1.04E-2</v>
+        <v>1.5800000000000002E-2</v>
       </c>
       <c r="I32" s="1"/>
       <c r="P32" s="10">
         <f>'VNINDEX T11-T12'!D27</f>
-        <v>1.04E-2</v>
+        <v>1.5800000000000002E-2</v>
       </c>
       <c r="Q32" s="1"/>
       <c r="X32" s="10">
         <f>'VNINDEX T11-T12'!D27</f>
-        <v>1.04E-2</v>
+        <v>1.5800000000000002E-2</v>
       </c>
       <c r="Y32" s="1"/>
       <c r="AF32" s="10">
         <f>'VNINDEX T11-T12'!D27</f>
-        <v>1.04E-2</v>
+        <v>1.5800000000000002E-2</v>
       </c>
       <c r="AG32" s="1"/>
       <c r="AN32" s="10">
         <f>'VNINDEX T11-T12'!D27</f>
-        <v>1.04E-2</v>
+        <v>1.5800000000000002E-2</v>
       </c>
       <c r="AO32" s="1"/>
       <c r="AV32" s="10">
         <f>'VNINDEX T11-T12'!D27</f>
-        <v>1.04E-2</v>
+        <v>1.5800000000000002E-2</v>
       </c>
       <c r="AW32" s="1"/>
       <c r="BD32" s="10">
         <f>'VNINDEX T11-T12'!D27</f>
-        <v>1.04E-2</v>
+        <v>1.5800000000000002E-2</v>
       </c>
       <c r="BE32" s="1"/>
       <c r="BL32" s="10">
         <f>'VNINDEX T11-T12'!D27</f>
-        <v>1.04E-2</v>
+        <v>1.5800000000000002E-2</v>
       </c>
       <c r="BM32" s="1"/>
       <c r="BT32" s="10">
         <f>'VNINDEX T11-T12'!D27</f>
-        <v>1.04E-2</v>
+        <v>1.5800000000000002E-2</v>
       </c>
       <c r="BU32" s="1"/>
       <c r="CB32" s="10">
         <f>'VNINDEX T11-T12'!D27</f>
-        <v>1.04E-2</v>
+        <v>1.5800000000000002E-2</v>
       </c>
       <c r="CC32" s="1"/>
       <c r="CJ32" s="10">
         <f>'VNINDEX T11-T12'!D27</f>
-        <v>1.04E-2</v>
+        <v>1.5800000000000002E-2</v>
       </c>
       <c r="CK32" s="1"/>
       <c r="CR32" s="10">
         <f>'VNINDEX T11-T12'!D27</f>
-        <v>1.04E-2</v>
+        <v>1.5800000000000002E-2</v>
       </c>
       <c r="CS32" s="1"/>
       <c r="CZ32" s="10">
         <f>'VNINDEX T11-T12'!D27</f>
-        <v>1.04E-2</v>
+        <v>1.5800000000000002E-2</v>
       </c>
       <c r="DA32" s="1"/>
       <c r="DH32" s="10">
         <f>'VNINDEX T11-T12'!D27</f>
-        <v>1.04E-2</v>
+        <v>1.5800000000000002E-2</v>
       </c>
       <c r="DI32" s="1"/>
       <c r="DP32" s="10">
         <f>'VNINDEX T11-T12'!D27</f>
-        <v>1.04E-2</v>
+        <v>1.5800000000000002E-2</v>
       </c>
       <c r="DQ32" s="1"/>
       <c r="DX32" s="10">
         <f>'VNINDEX T11-T12'!D27</f>
-        <v>1.04E-2</v>
+        <v>1.5800000000000002E-2</v>
       </c>
       <c r="DY32" s="1"/>
       <c r="EF32" s="10">
         <f>'VNINDEX T11-T12'!D27</f>
-        <v>1.04E-2</v>
+        <v>1.5800000000000002E-2</v>
       </c>
       <c r="EG32" s="1"/>
       <c r="EN32" s="10">
         <f>'VNINDEX T11-T12'!D27</f>
-        <v>1.04E-2</v>
+        <v>1.5800000000000002E-2</v>
       </c>
       <c r="EO32" s="1"/>
       <c r="EV32" s="10">
         <f>'VNINDEX T11-T12'!D27</f>
-        <v>1.04E-2</v>
+        <v>1.5800000000000002E-2</v>
       </c>
       <c r="EW32" s="1"/>
       <c r="FD32" s="10">
         <f>'VNINDEX T11-T12'!D27</f>
-        <v>1.04E-2</v>
+        <v>1.5800000000000002E-2</v>
       </c>
       <c r="FE32" s="1"/>
       <c r="FL32" s="10">
         <f>'VNINDEX T11-T12'!D27</f>
-        <v>1.04E-2</v>
+        <v>1.5800000000000002E-2</v>
       </c>
       <c r="FM32" s="1"/>
       <c r="FT32" s="10">
         <f>'VNINDEX T11-T12'!D27</f>
-        <v>1.04E-2</v>
+        <v>1.5800000000000002E-2</v>
       </c>
       <c r="FU32" s="1"/>
     </row>
@@ -11713,7 +11984,22 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="33">
+  <mergeCells count="31">
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="BF1:CB1"/>
+    <mergeCell ref="CD1:DP1"/>
+    <mergeCell ref="DR1:EF1"/>
+    <mergeCell ref="DZ2:EF2"/>
+    <mergeCell ref="CT2:CZ2"/>
+    <mergeCell ref="DB2:DH2"/>
+    <mergeCell ref="DJ2:DP2"/>
+    <mergeCell ref="AX2:BD2"/>
+    <mergeCell ref="BF2:BK2"/>
+    <mergeCell ref="BN2:BT2"/>
+    <mergeCell ref="EX1:FD1"/>
+    <mergeCell ref="CL2:CR2"/>
+    <mergeCell ref="DR2:DX2"/>
+    <mergeCell ref="EH1:EV1"/>
     <mergeCell ref="FF1:FL1"/>
     <mergeCell ref="BV2:CB2"/>
     <mergeCell ref="FN1:FT1"/>
@@ -11730,23 +12016,6 @@
     <mergeCell ref="FN2:FT2"/>
     <mergeCell ref="CD2:CJ2"/>
     <mergeCell ref="EH2:EN2"/>
-    <mergeCell ref="EX1:FD1"/>
-    <mergeCell ref="B2:H2"/>
-    <mergeCell ref="CL2:CR2"/>
-    <mergeCell ref="DR2:DX2"/>
-    <mergeCell ref="EH1:EV1"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="BF1:CB1"/>
-    <mergeCell ref="CD1:DP1"/>
-    <mergeCell ref="DR1:EF1"/>
-    <mergeCell ref="DZ2:EF2"/>
-    <mergeCell ref="B1:P1"/>
-    <mergeCell ref="CT2:CZ2"/>
-    <mergeCell ref="DB2:DH2"/>
-    <mergeCell ref="DJ2:DP2"/>
-    <mergeCell ref="AX2:BD2"/>
-    <mergeCell ref="BF2:BK2"/>
-    <mergeCell ref="BN2:BT2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -11755,38 +12024,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44AE7D72-BA61-2B48-B575-56ABA60372B7}">
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D27" sqref="D27"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13.6640625" customWidth="1"/>
-    <col min="6" max="6" width="13.5" customWidth="1"/>
-    <col min="7" max="7" width="18.5" customWidth="1"/>
-    <col min="8" max="8" width="16.83203125" customWidth="1"/>
+    <col min="6" max="6" width="18.5" customWidth="1"/>
+    <col min="7" max="7" width="16.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="13"/>
-      <c r="B1" s="97" t="s">
+      <c r="B1" s="51" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="97"/>
-      <c r="D1" s="97"/>
-      <c r="E1" s="97"/>
-      <c r="F1" s="97"/>
-      <c r="G1" s="97"/>
-      <c r="H1" s="97"/>
-      <c r="I1" s="97"/>
-      <c r="J1" s="97"/>
-      <c r="K1" s="97"/>
-      <c r="L1" s="97"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>31</v>
       </c>
@@ -11820,11 +12086,8 @@
       <c r="K2" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>57</v>
-      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="16">
         <v>45245</v>
       </c>
@@ -11841,22 +12104,19 @@
         <v>1.47E-2</v>
       </c>
       <c r="F3" s="6">
-        <v>11317236</v>
+        <v>244955370000</v>
       </c>
       <c r="G3" s="6">
-        <v>244955370000</v>
-      </c>
-      <c r="H3" s="6">
         <v>937960012</v>
       </c>
-      <c r="I3" s="26" t="s">
-        <v>62</v>
-      </c>
+      <c r="H3" s="26" t="s">
+        <v>60</v>
+      </c>
+      <c r="I3" s="12"/>
       <c r="J3" s="12"/>
-      <c r="K3" s="12"/>
-      <c r="L3" s="28"/>
+      <c r="K3" s="28"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="16">
         <v>45246</v>
       </c>
@@ -11873,22 +12133,19 @@
         <v>8.9999999999999993E-3</v>
       </c>
       <c r="F4" s="6">
-        <v>-4974264</v>
+        <v>-130199340000</v>
       </c>
       <c r="G4" s="6">
-        <v>-130199340000</v>
-      </c>
-      <c r="H4" s="6">
         <v>687396150</v>
       </c>
-      <c r="I4" s="26" t="s">
-        <v>63</v>
-      </c>
+      <c r="H4" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="I4" s="12"/>
       <c r="J4" s="12"/>
-      <c r="K4" s="12"/>
-      <c r="L4" s="28"/>
+      <c r="K4" s="28"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="16">
         <v>45247</v>
       </c>
@@ -11905,22 +12162,19 @@
         <v>2.93E-2</v>
       </c>
       <c r="F5" s="6">
-        <v>-31139110</v>
+        <v>-749187610000</v>
       </c>
       <c r="G5" s="6">
-        <v>-749187610000</v>
-      </c>
-      <c r="H5" s="6">
         <v>1255204381</v>
       </c>
-      <c r="I5" s="26" t="s">
-        <v>64</v>
-      </c>
+      <c r="H5" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="I5" s="12"/>
       <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="28"/>
+      <c r="K5" s="28"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="16">
         <v>45250</v>
       </c>
@@ -11937,22 +12191,19 @@
         <v>2.3E-2</v>
       </c>
       <c r="F6" s="6">
-        <v>15889449</v>
+        <v>465544880000</v>
       </c>
       <c r="G6" s="6">
-        <v>465544880000</v>
-      </c>
-      <c r="H6" s="6">
         <v>841468794</v>
       </c>
-      <c r="I6" s="26" t="s">
-        <v>65</v>
-      </c>
+      <c r="H6" s="26" t="s">
+        <v>63</v>
+      </c>
+      <c r="I6" s="12"/>
       <c r="J6" s="12"/>
-      <c r="K6" s="12"/>
-      <c r="L6" s="28"/>
+      <c r="K6" s="28"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="16">
         <v>45251</v>
       </c>
@@ -11969,22 +12220,19 @@
         <v>8.0000000000000002E-3</v>
       </c>
       <c r="F7" s="6">
-        <v>-25881982</v>
+        <v>-581773030000</v>
       </c>
       <c r="G7" s="6">
-        <v>-581773030000</v>
-      </c>
-      <c r="H7" s="6">
         <v>712613814</v>
       </c>
-      <c r="I7" s="26" t="s">
-        <v>66</v>
-      </c>
+      <c r="H7" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="I7" s="12"/>
       <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="28"/>
+      <c r="K7" s="28"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="16">
         <v>45252</v>
       </c>
@@ -12001,22 +12249,19 @@
         <v>1.0800000000000001E-2</v>
       </c>
       <c r="F8" s="6">
-        <v>-31243345</v>
+        <v>-746289940000</v>
       </c>
       <c r="G8" s="6">
-        <v>-746289940000</v>
-      </c>
-      <c r="H8" s="6">
         <v>946276924</v>
       </c>
-      <c r="I8" s="26" t="s">
-        <v>67</v>
-      </c>
+      <c r="H8" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="I8" s="12"/>
       <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="28"/>
+      <c r="K8" s="28"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="16">
         <v>45253</v>
       </c>
@@ -12033,22 +12278,19 @@
         <v>2.6800000000000001E-2</v>
       </c>
       <c r="F9" s="6">
-        <v>-16124265</v>
+        <v>-445810740000</v>
       </c>
       <c r="G9" s="6">
-        <v>-445810740000</v>
-      </c>
-      <c r="H9" s="6">
         <v>1028270888</v>
       </c>
-      <c r="I9" s="26" t="s">
-        <v>68</v>
-      </c>
+      <c r="H9" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="I9" s="12"/>
       <c r="J9" s="12"/>
-      <c r="K9" s="12"/>
-      <c r="L9" s="28"/>
+      <c r="K9" s="28"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="16">
         <v>45254</v>
       </c>
@@ -12065,28 +12307,25 @@
         <v>2.06E-2</v>
       </c>
       <c r="F10" s="6">
-        <v>8243442</v>
+        <v>398629530000</v>
       </c>
       <c r="G10" s="6">
-        <v>398629530000</v>
-      </c>
-      <c r="H10" s="6">
         <v>958343250</v>
       </c>
-      <c r="I10" s="26" t="s">
-        <v>69</v>
+      <c r="H10" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="I10" s="32">
+        <v>146</v>
       </c>
       <c r="J10" s="32">
-        <v>146</v>
-      </c>
-      <c r="K10" s="32">
         <v>77</v>
       </c>
-      <c r="L10" s="29">
+      <c r="K10" s="29">
         <v>381</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="16">
         <v>45257</v>
       </c>
@@ -12103,28 +12342,25 @@
         <v>0.01</v>
       </c>
       <c r="F11" s="6">
-        <v>713470</v>
+        <v>40538100000</v>
       </c>
       <c r="G11" s="6">
-        <v>40538100000</v>
-      </c>
-      <c r="H11" s="6">
         <v>595015273</v>
       </c>
-      <c r="I11" s="26" t="s">
-        <v>70</v>
+      <c r="H11" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="I11" s="12">
+        <v>165</v>
       </c>
       <c r="J11" s="12">
-        <v>165</v>
-      </c>
-      <c r="K11" s="12">
         <v>85</v>
       </c>
-      <c r="L11" s="28">
+      <c r="K11" s="28">
         <v>351</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="16">
         <v>45258</v>
       </c>
@@ -12141,28 +12377,25 @@
         <v>1.7500000000000002E-2</v>
       </c>
       <c r="F12" s="6">
-        <v>1657959</v>
+        <v>48002310000</v>
       </c>
       <c r="G12" s="6">
-        <v>48002310000</v>
-      </c>
-      <c r="H12" s="6">
         <v>681884567</v>
       </c>
-      <c r="I12" s="26" t="s">
-        <v>71</v>
+      <c r="H12" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="I12" s="12">
+        <v>290</v>
       </c>
       <c r="J12" s="12">
-        <v>290</v>
-      </c>
-      <c r="K12" s="12">
         <v>100</v>
       </c>
-      <c r="L12" s="28">
+      <c r="K12" s="28">
         <v>210</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="16">
         <v>45259</v>
       </c>
@@ -12179,28 +12412,25 @@
         <v>8.0999999999999996E-3</v>
       </c>
       <c r="F13" s="6">
-        <v>-5560500</v>
+        <v>-100710330000</v>
       </c>
       <c r="G13" s="6">
-        <v>-100710330000</v>
-      </c>
-      <c r="H13" s="6">
         <v>614957140</v>
       </c>
-      <c r="I13" s="26" t="s">
-        <v>72</v>
+      <c r="H13" s="26" t="s">
+        <v>70</v>
+      </c>
+      <c r="I13" s="12">
+        <v>383</v>
       </c>
       <c r="J13" s="12">
-        <v>383</v>
-      </c>
-      <c r="K13" s="12">
         <v>97</v>
       </c>
-      <c r="L13" s="28">
+      <c r="K13" s="28">
         <v>122</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="16">
         <v>45260</v>
       </c>
@@ -12217,28 +12447,25 @@
         <v>1.2E-2</v>
       </c>
       <c r="F14" s="6">
-        <v>-5540455</v>
+        <v>-383361210000</v>
       </c>
       <c r="G14" s="6">
-        <v>-383361210000</v>
-      </c>
-      <c r="H14" s="6">
         <v>723483378</v>
       </c>
-      <c r="I14" s="26" t="s">
-        <v>73</v>
+      <c r="H14" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="I14" s="12">
+        <v>138</v>
       </c>
       <c r="J14" s="12">
-        <v>138</v>
-      </c>
-      <c r="K14" s="12">
         <v>134</v>
       </c>
-      <c r="L14" s="28">
+      <c r="K14" s="28">
         <v>374</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="19">
         <v>45261</v>
       </c>
@@ -12255,28 +12482,25 @@
         <v>1.0699999999999999E-2</v>
       </c>
       <c r="F15" s="6">
-        <v>-12769030</v>
+        <v>-309034110000</v>
       </c>
       <c r="G15" s="6">
-        <v>-309034110000</v>
-      </c>
-      <c r="H15" s="6">
         <v>603587510</v>
       </c>
-      <c r="I15" s="26" t="s">
-        <v>74</v>
+      <c r="H15" s="26" t="s">
+        <v>72</v>
+      </c>
+      <c r="I15" s="12">
+        <v>254</v>
       </c>
       <c r="J15" s="12">
-        <v>254</v>
-      </c>
-      <c r="K15" s="12">
         <v>101</v>
       </c>
-      <c r="L15" s="28">
+      <c r="K15" s="28">
         <v>227</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="19">
         <v>45264</v>
       </c>
@@ -12293,60 +12517,95 @@
         <v>1.5599999999999999E-2</v>
       </c>
       <c r="F16" s="6">
-        <v>-20786620</v>
+        <v>-582719066595.16309</v>
       </c>
       <c r="G16" s="6">
-        <v>-582719066595.16309</v>
-      </c>
-      <c r="H16" s="6">
         <v>1120648335</v>
       </c>
-      <c r="I16" s="26" t="s">
-        <v>75</v>
+      <c r="H16" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="I16" s="12">
+        <v>487</v>
       </c>
       <c r="J16" s="12">
-        <v>487</v>
-      </c>
-      <c r="K16" s="12">
         <v>56</v>
       </c>
-      <c r="L16" s="28">
+      <c r="K16" s="28">
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="19">
         <v>45265</v>
       </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="28"/>
+      <c r="B17" s="6">
+        <v>1115.97</v>
+      </c>
+      <c r="C17" s="17">
+        <v>-4.5199999999999996</v>
+      </c>
+      <c r="D17" s="18">
+        <v>-4.0000000000000001E-3</v>
+      </c>
+      <c r="E17" s="18">
+        <v>0.01</v>
+      </c>
+      <c r="F17" s="6">
+        <v>-1557712480000</v>
+      </c>
+      <c r="G17" s="6">
+        <v>824655978</v>
+      </c>
+      <c r="H17" s="10">
+        <v>0.12543841887968463</v>
+      </c>
+      <c r="I17" s="12">
+        <v>141</v>
+      </c>
+      <c r="J17" s="12">
+        <v>96</v>
+      </c>
+      <c r="K17" s="28">
+        <v>356</v>
+      </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="19">
         <v>45266</v>
       </c>
-      <c r="B18" s="6"/>
-      <c r="C18" s="17"/>
-      <c r="D18" s="18"/>
-      <c r="E18" s="18"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="28"/>
+      <c r="B18" s="6">
+        <v>1126.43</v>
+      </c>
+      <c r="C18" s="17">
+        <v>10.46</v>
+      </c>
+      <c r="D18" s="18">
+        <v>9.4000000000000004E-3</v>
+      </c>
+      <c r="E18" s="18">
+        <v>9.2999999999999992E-3</v>
+      </c>
+      <c r="F18" s="6">
+        <v>-548607720000</v>
+      </c>
+      <c r="G18" s="6">
+        <v>853960306</v>
+      </c>
+      <c r="H18" s="10">
+        <v>0.12706528422645444</v>
+      </c>
+      <c r="I18" s="12">
+        <v>359</v>
+      </c>
+      <c r="J18" s="12">
+        <v>92</v>
+      </c>
+      <c r="K18" s="28">
+        <v>122</v>
+      </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="19">
         <v>45267</v>
       </c>
@@ -12356,13 +12615,12 @@
       <c r="E19" s="18"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="26"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="12"/>
       <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="28"/>
+      <c r="K19" s="28"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="19">
         <v>45268</v>
       </c>
@@ -12372,13 +12630,12 @@
       <c r="E20" s="18"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="26"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="12"/>
       <c r="J20" s="12"/>
-      <c r="K20" s="12"/>
-      <c r="L20" s="28"/>
+      <c r="K20" s="28"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="19">
         <v>45271</v>
       </c>
@@ -12388,13 +12645,12 @@
       <c r="E21" s="18"/>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="12"/>
       <c r="J21" s="12"/>
-      <c r="K21" s="12"/>
-      <c r="L21" s="28"/>
+      <c r="K21" s="28"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="19">
         <v>45272</v>
       </c>
@@ -12404,13 +12660,12 @@
       <c r="E22" s="18"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="26"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="12"/>
       <c r="J22" s="12"/>
-      <c r="K22" s="12"/>
-      <c r="L22" s="28"/>
+      <c r="K22" s="28"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="19">
         <v>45273</v>
       </c>
@@ -12420,13 +12675,12 @@
       <c r="E23" s="18"/>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="26"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="12"/>
       <c r="J23" s="12"/>
-      <c r="K23" s="12"/>
-      <c r="L23" s="28"/>
+      <c r="K23" s="28"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="19">
         <v>45274</v>
       </c>
@@ -12436,13 +12690,12 @@
       <c r="E24" s="18"/>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="26"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="12"/>
       <c r="J24" s="12"/>
-      <c r="K24" s="12"/>
-      <c r="L24" s="28"/>
+      <c r="K24" s="28"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="20">
         <v>45275</v>
       </c>
@@ -12452,62 +12705,67 @@
       <c r="E25" s="23"/>
       <c r="F25" s="21"/>
       <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="27"/>
+      <c r="H25" s="27"/>
+      <c r="I25" s="24"/>
       <c r="J25" s="24"/>
-      <c r="K25" s="24"/>
-      <c r="L25" s="33"/>
+      <c r="K25" s="33"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" s="9" t="s">
-        <v>58</v>
-      </c>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="52" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" s="52"/>
       <c r="C27" s="25">
         <f>SUM(C3:C25)</f>
-        <v>10.76</v>
+        <v>16.700000000000003</v>
       </c>
       <c r="D27" s="10">
         <f>SUM(D3:D25)</f>
-        <v>1.04E-2</v>
+        <v>1.5800000000000002E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" s="9" t="s">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="B28" s="52"/>
+      <c r="G28" s="6">
+        <f>AVERAGE(G3:G25)</f>
+        <v>835451092.93333328</v>
+      </c>
+      <c r="H28" s="6"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" s="52" t="s">
         <v>59</v>
       </c>
-      <c r="H28" s="6">
-        <f>AVERAGE(H3:H25)</f>
-        <v>836222172.57142854</v>
-      </c>
-      <c r="I28" s="6"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29" s="9" t="s">
-        <v>60</v>
-      </c>
+      <c r="B29" s="52"/>
       <c r="E29" s="10">
         <f>AVERAGE(E3:E25)</f>
-        <v>1.5435714285714287E-2</v>
+        <v>1.4712500000000002E-2</v>
       </c>
       <c r="F29" s="10"/>
-      <c r="G29" s="10"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A30" s="9" t="s">
-        <v>61</v>
-      </c>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="B30" s="52"/>
       <c r="F30" s="6">
         <f>SUM(F3:F25)</f>
-        <v>-116198015</v>
+        <v>-4389127666595.1631</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:L1"/>
+  <mergeCells count="5">
+    <mergeCell ref="B1:K1"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
cap nhat ngay 7/12/2023
</commit_message>
<xml_diff>
--- a/2023/DongTien-T11-T12.xlsx
+++ b/2023/DongTien-T11-T12.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trung.nguyenhoang/stocks/2023/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/Desktop/stocks/2023/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10CE1756-954E-5D4F-A056-1C3033B00A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE0C2FC6-DB4C-6C43-99BA-D90CD114CCA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17060" xr2:uid="{B7EC2610-802E-D441-AB46-76A27057AA52}"/>
   </bookViews>
@@ -16,16 +16,6 @@
     <sheet name="GDNN T11-T12" sheetId="1" r:id="rId1"/>
     <sheet name="VNINDEX T11-T12" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.4" hidden="1">'GDNN T11-T12'!$A$4:$A$19</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'GDNN T11-T12'!$B$4:$B$19</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'GDNN T11-T12'!$C$4:$C$19</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'GDNN T11-T12'!$D$4:$D$19</definedName>
-    <definedName name="_xlchart.v2.0" hidden="1">'GDNN T11-T12'!$A$4:$A$19</definedName>
-    <definedName name="_xlchart.v2.1" hidden="1">'GDNN T11-T12'!$B$4:$B$19</definedName>
-    <definedName name="_xlchart.v2.2" hidden="1">'GDNN T11-T12'!$C$4:$C$19</definedName>
-    <definedName name="_xlchart.v2.3" hidden="1">'GDNN T11-T12'!$D$4:$D$19</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -281,7 +271,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -319,8 +309,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -397,6 +401,16 @@
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -527,11 +541,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -578,27 +594,52 @@
     </xf>
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -611,10 +652,31 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -623,10 +685,12 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="5" fillId="14" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="6" fillId="15" borderId="0" xfId="3" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
@@ -943,8 +1007,8 @@
   <dimension ref="A1:FU39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E16" sqref="E16"/>
+      <pane xSplit="1" topLeftCell="FD1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="DN20" sqref="DN20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -958,7 +1022,7 @@
     <col min="7" max="7" width="11.5" customWidth="1"/>
     <col min="13" max="13" width="17.5" customWidth="1"/>
     <col min="14" max="14" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="14.1640625" customWidth="1"/>
+    <col min="21" max="21" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="13.6640625" customWidth="1"/>
     <col min="29" max="29" width="15.1640625" customWidth="1"/>
     <col min="37" max="37" width="16" customWidth="1"/>
@@ -987,431 +1051,431 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:177" x14ac:dyDescent="0.2">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="84" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
       <c r="Q1" s="1"/>
-      <c r="R1" s="41" t="s">
+      <c r="R1" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="S1" s="41"/>
-      <c r="T1" s="41"/>
-      <c r="U1" s="41"/>
-      <c r="V1" s="41"/>
-      <c r="W1" s="41"/>
-      <c r="X1" s="41"/>
-      <c r="Y1" s="41"/>
-      <c r="Z1" s="41"/>
-      <c r="AA1" s="41"/>
-      <c r="AB1" s="41"/>
-      <c r="AC1" s="41"/>
-      <c r="AD1" s="41"/>
-      <c r="AE1" s="41"/>
-      <c r="AF1" s="41"/>
-      <c r="AG1" s="41"/>
-      <c r="AH1" s="41"/>
-      <c r="AI1" s="41"/>
-      <c r="AJ1" s="41"/>
-      <c r="AK1" s="41"/>
-      <c r="AL1" s="41"/>
-      <c r="AM1" s="41"/>
-      <c r="AN1" s="41"/>
-      <c r="AO1" s="42" t="s">
+      <c r="S1" s="95"/>
+      <c r="T1" s="95"/>
+      <c r="U1" s="95"/>
+      <c r="V1" s="95"/>
+      <c r="W1" s="95"/>
+      <c r="X1" s="95"/>
+      <c r="Y1" s="95"/>
+      <c r="Z1" s="95"/>
+      <c r="AA1" s="95"/>
+      <c r="AB1" s="95"/>
+      <c r="AC1" s="95"/>
+      <c r="AD1" s="95"/>
+      <c r="AE1" s="95"/>
+      <c r="AF1" s="95"/>
+      <c r="AG1" s="95"/>
+      <c r="AH1" s="95"/>
+      <c r="AI1" s="95"/>
+      <c r="AJ1" s="95"/>
+      <c r="AK1" s="95"/>
+      <c r="AL1" s="95"/>
+      <c r="AM1" s="95"/>
+      <c r="AN1" s="95"/>
+      <c r="AO1" s="96" t="s">
         <v>2</v>
       </c>
-      <c r="AP1" s="42"/>
-      <c r="AQ1" s="42"/>
-      <c r="AR1" s="42"/>
-      <c r="AS1" s="42"/>
-      <c r="AT1" s="42"/>
-      <c r="AU1" s="42"/>
-      <c r="AV1" s="42"/>
-      <c r="AW1" s="42"/>
-      <c r="AX1" s="42"/>
-      <c r="AY1" s="42"/>
-      <c r="AZ1" s="42"/>
-      <c r="BA1" s="42"/>
-      <c r="BB1" s="42"/>
-      <c r="BC1" s="42"/>
+      <c r="AP1" s="96"/>
+      <c r="AQ1" s="96"/>
+      <c r="AR1" s="96"/>
+      <c r="AS1" s="96"/>
+      <c r="AT1" s="96"/>
+      <c r="AU1" s="96"/>
+      <c r="AV1" s="96"/>
+      <c r="AW1" s="96"/>
+      <c r="AX1" s="96"/>
+      <c r="AY1" s="96"/>
+      <c r="AZ1" s="96"/>
+      <c r="BA1" s="96"/>
+      <c r="BB1" s="96"/>
+      <c r="BC1" s="96"/>
       <c r="BD1" s="1"/>
       <c r="BE1" s="1"/>
-      <c r="BF1" s="46" t="s">
+      <c r="BF1" s="85" t="s">
         <v>46</v>
       </c>
-      <c r="BG1" s="46"/>
-      <c r="BH1" s="46"/>
-      <c r="BI1" s="46"/>
-      <c r="BJ1" s="46"/>
-      <c r="BK1" s="46"/>
-      <c r="BL1" s="46"/>
-      <c r="BM1" s="46"/>
-      <c r="BN1" s="46"/>
-      <c r="BO1" s="46"/>
-      <c r="BP1" s="46"/>
-      <c r="BQ1" s="46"/>
-      <c r="BR1" s="46"/>
-      <c r="BS1" s="46"/>
-      <c r="BT1" s="46"/>
-      <c r="BU1" s="46"/>
-      <c r="BV1" s="46"/>
-      <c r="BW1" s="46"/>
-      <c r="BX1" s="46"/>
-      <c r="BY1" s="46"/>
-      <c r="BZ1" s="46"/>
-      <c r="CA1" s="46"/>
-      <c r="CB1" s="46"/>
+      <c r="BG1" s="85"/>
+      <c r="BH1" s="85"/>
+      <c r="BI1" s="85"/>
+      <c r="BJ1" s="85"/>
+      <c r="BK1" s="85"/>
+      <c r="BL1" s="85"/>
+      <c r="BM1" s="85"/>
+      <c r="BN1" s="85"/>
+      <c r="BO1" s="85"/>
+      <c r="BP1" s="85"/>
+      <c r="BQ1" s="85"/>
+      <c r="BR1" s="85"/>
+      <c r="BS1" s="85"/>
+      <c r="BT1" s="85"/>
+      <c r="BU1" s="85"/>
+      <c r="BV1" s="85"/>
+      <c r="BW1" s="85"/>
+      <c r="BX1" s="85"/>
+      <c r="BY1" s="85"/>
+      <c r="BZ1" s="85"/>
+      <c r="CA1" s="85"/>
+      <c r="CB1" s="85"/>
       <c r="CC1" s="1"/>
-      <c r="CD1" s="47" t="s">
+      <c r="CD1" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="CE1" s="47"/>
-      <c r="CF1" s="47"/>
-      <c r="CG1" s="47"/>
-      <c r="CH1" s="47"/>
-      <c r="CI1" s="47"/>
-      <c r="CJ1" s="47"/>
-      <c r="CK1" s="47"/>
-      <c r="CL1" s="47"/>
-      <c r="CM1" s="47"/>
-      <c r="CN1" s="47"/>
-      <c r="CO1" s="47"/>
-      <c r="CP1" s="47"/>
-      <c r="CQ1" s="47"/>
-      <c r="CR1" s="47"/>
-      <c r="CS1" s="47"/>
-      <c r="CT1" s="47"/>
-      <c r="CU1" s="47"/>
-      <c r="CV1" s="47"/>
-      <c r="CW1" s="47"/>
-      <c r="CX1" s="47"/>
-      <c r="CY1" s="47"/>
-      <c r="CZ1" s="47"/>
-      <c r="DA1" s="47"/>
-      <c r="DB1" s="47"/>
-      <c r="DC1" s="47"/>
-      <c r="DD1" s="47"/>
-      <c r="DE1" s="47"/>
-      <c r="DF1" s="47"/>
-      <c r="DG1" s="47"/>
-      <c r="DH1" s="47"/>
-      <c r="DI1" s="47"/>
-      <c r="DJ1" s="47"/>
-      <c r="DK1" s="47"/>
-      <c r="DL1" s="47"/>
-      <c r="DM1" s="47"/>
-      <c r="DN1" s="47"/>
-      <c r="DO1" s="47"/>
-      <c r="DP1" s="47"/>
+      <c r="CE1" s="86"/>
+      <c r="CF1" s="86"/>
+      <c r="CG1" s="86"/>
+      <c r="CH1" s="86"/>
+      <c r="CI1" s="86"/>
+      <c r="CJ1" s="86"/>
+      <c r="CK1" s="86"/>
+      <c r="CL1" s="86"/>
+      <c r="CM1" s="86"/>
+      <c r="CN1" s="86"/>
+      <c r="CO1" s="86"/>
+      <c r="CP1" s="86"/>
+      <c r="CQ1" s="86"/>
+      <c r="CR1" s="86"/>
+      <c r="CS1" s="86"/>
+      <c r="CT1" s="86"/>
+      <c r="CU1" s="86"/>
+      <c r="CV1" s="86"/>
+      <c r="CW1" s="86"/>
+      <c r="CX1" s="86"/>
+      <c r="CY1" s="86"/>
+      <c r="CZ1" s="86"/>
+      <c r="DA1" s="86"/>
+      <c r="DB1" s="86"/>
+      <c r="DC1" s="86"/>
+      <c r="DD1" s="86"/>
+      <c r="DE1" s="86"/>
+      <c r="DF1" s="86"/>
+      <c r="DG1" s="86"/>
+      <c r="DH1" s="86"/>
+      <c r="DI1" s="86"/>
+      <c r="DJ1" s="86"/>
+      <c r="DK1" s="86"/>
+      <c r="DL1" s="86"/>
+      <c r="DM1" s="86"/>
+      <c r="DN1" s="86"/>
+      <c r="DO1" s="86"/>
+      <c r="DP1" s="86"/>
       <c r="DQ1" s="1"/>
-      <c r="DR1" s="48" t="s">
+      <c r="DR1" s="87" t="s">
         <v>4</v>
       </c>
-      <c r="DS1" s="48"/>
-      <c r="DT1" s="48"/>
-      <c r="DU1" s="48"/>
-      <c r="DV1" s="48"/>
-      <c r="DW1" s="48"/>
-      <c r="DX1" s="48"/>
-      <c r="DY1" s="48"/>
-      <c r="DZ1" s="48"/>
-      <c r="EA1" s="48"/>
-      <c r="EB1" s="48"/>
-      <c r="EC1" s="48"/>
-      <c r="ED1" s="48"/>
-      <c r="EE1" s="48"/>
-      <c r="EF1" s="48"/>
+      <c r="DS1" s="87"/>
+      <c r="DT1" s="87"/>
+      <c r="DU1" s="87"/>
+      <c r="DV1" s="87"/>
+      <c r="DW1" s="87"/>
+      <c r="DX1" s="87"/>
+      <c r="DY1" s="87"/>
+      <c r="DZ1" s="87"/>
+      <c r="EA1" s="87"/>
+      <c r="EB1" s="87"/>
+      <c r="EC1" s="87"/>
+      <c r="ED1" s="87"/>
+      <c r="EE1" s="87"/>
+      <c r="EF1" s="87"/>
       <c r="EG1" s="1"/>
-      <c r="EH1" s="44" t="s">
+      <c r="EH1" s="92" t="s">
         <v>5</v>
       </c>
-      <c r="EI1" s="44"/>
-      <c r="EJ1" s="44"/>
-      <c r="EK1" s="44"/>
-      <c r="EL1" s="44"/>
-      <c r="EM1" s="44"/>
-      <c r="EN1" s="44"/>
-      <c r="EO1" s="44"/>
-      <c r="EP1" s="44"/>
-      <c r="EQ1" s="44"/>
-      <c r="ER1" s="44"/>
-      <c r="ES1" s="44"/>
-      <c r="ET1" s="44"/>
-      <c r="EU1" s="44"/>
-      <c r="EV1" s="44"/>
+      <c r="EI1" s="92"/>
+      <c r="EJ1" s="92"/>
+      <c r="EK1" s="92"/>
+      <c r="EL1" s="92"/>
+      <c r="EM1" s="92"/>
+      <c r="EN1" s="92"/>
+      <c r="EO1" s="92"/>
+      <c r="EP1" s="92"/>
+      <c r="EQ1" s="92"/>
+      <c r="ER1" s="92"/>
+      <c r="ES1" s="92"/>
+      <c r="ET1" s="92"/>
+      <c r="EU1" s="92"/>
+      <c r="EV1" s="92"/>
       <c r="EW1" s="1"/>
-      <c r="EX1" s="43" t="s">
+      <c r="EX1" s="91" t="s">
         <v>6</v>
       </c>
-      <c r="EY1" s="43"/>
-      <c r="EZ1" s="43"/>
-      <c r="FA1" s="43"/>
-      <c r="FB1" s="43"/>
-      <c r="FC1" s="43"/>
-      <c r="FD1" s="43"/>
+      <c r="EY1" s="91"/>
+      <c r="EZ1" s="91"/>
+      <c r="FA1" s="91"/>
+      <c r="FB1" s="91"/>
+      <c r="FC1" s="91"/>
+      <c r="FD1" s="91"/>
       <c r="FE1" s="1"/>
-      <c r="FF1" s="38" t="s">
+      <c r="FF1" s="93" t="s">
         <v>7</v>
       </c>
-      <c r="FG1" s="38"/>
-      <c r="FH1" s="38"/>
-      <c r="FI1" s="38"/>
-      <c r="FJ1" s="38"/>
-      <c r="FK1" s="38"/>
-      <c r="FL1" s="38"/>
+      <c r="FG1" s="93"/>
+      <c r="FH1" s="93"/>
+      <c r="FI1" s="93"/>
+      <c r="FJ1" s="93"/>
+      <c r="FK1" s="93"/>
+      <c r="FL1" s="93"/>
       <c r="FM1" s="1"/>
-      <c r="FN1" s="40" t="s">
+      <c r="FN1" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="FO1" s="40"/>
-      <c r="FP1" s="40"/>
-      <c r="FQ1" s="40"/>
-      <c r="FR1" s="40"/>
-      <c r="FS1" s="40"/>
-      <c r="FT1" s="40"/>
+      <c r="FO1" s="94"/>
+      <c r="FP1" s="94"/>
+      <c r="FQ1" s="94"/>
+      <c r="FR1" s="94"/>
+      <c r="FS1" s="94"/>
+      <c r="FT1" s="94"/>
       <c r="FU1" s="1"/>
     </row>
     <row r="2" spans="1:177" x14ac:dyDescent="0.2">
-      <c r="A2" s="45"/>
-      <c r="B2" s="54" t="s">
+      <c r="A2" s="84"/>
+      <c r="B2" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
       <c r="I2" s="1"/>
-      <c r="J2" s="39" t="s">
+      <c r="J2" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="39"/>
-      <c r="P2" s="39"/>
+      <c r="K2" s="88"/>
+      <c r="L2" s="88"/>
+      <c r="M2" s="88"/>
+      <c r="N2" s="88"/>
+      <c r="O2" s="88"/>
+      <c r="P2" s="88"/>
       <c r="Q2" s="1"/>
-      <c r="R2" s="39" t="s">
+      <c r="R2" s="88" t="s">
         <v>11</v>
       </c>
-      <c r="S2" s="39"/>
-      <c r="T2" s="39"/>
-      <c r="U2" s="39"/>
-      <c r="V2" s="39"/>
-      <c r="W2" s="39"/>
-      <c r="X2" s="39"/>
+      <c r="S2" s="88"/>
+      <c r="T2" s="88"/>
+      <c r="U2" s="88"/>
+      <c r="V2" s="88"/>
+      <c r="W2" s="88"/>
+      <c r="X2" s="88"/>
       <c r="Y2" s="1"/>
-      <c r="Z2" s="39" t="s">
+      <c r="Z2" s="88" t="s">
         <v>12</v>
       </c>
-      <c r="AA2" s="39"/>
-      <c r="AB2" s="39"/>
-      <c r="AC2" s="39"/>
-      <c r="AD2" s="39"/>
-      <c r="AE2" s="39"/>
-      <c r="AF2" s="39"/>
+      <c r="AA2" s="88"/>
+      <c r="AB2" s="88"/>
+      <c r="AC2" s="88"/>
+      <c r="AD2" s="88"/>
+      <c r="AE2" s="88"/>
+      <c r="AF2" s="88"/>
       <c r="AG2" s="1"/>
-      <c r="AH2" s="39" t="s">
+      <c r="AH2" s="88" t="s">
         <v>13</v>
       </c>
-      <c r="AI2" s="39"/>
-      <c r="AJ2" s="39"/>
-      <c r="AK2" s="39"/>
-      <c r="AL2" s="39"/>
-      <c r="AM2" s="39"/>
-      <c r="AN2" s="39"/>
+      <c r="AI2" s="88"/>
+      <c r="AJ2" s="88"/>
+      <c r="AK2" s="88"/>
+      <c r="AL2" s="88"/>
+      <c r="AM2" s="88"/>
+      <c r="AN2" s="88"/>
       <c r="AO2" s="1"/>
-      <c r="AP2" s="39" t="s">
+      <c r="AP2" s="88" t="s">
         <v>14</v>
       </c>
-      <c r="AQ2" s="39"/>
-      <c r="AR2" s="39"/>
-      <c r="AS2" s="39"/>
-      <c r="AT2" s="39"/>
-      <c r="AU2" s="39"/>
-      <c r="AV2" s="39"/>
+      <c r="AQ2" s="88"/>
+      <c r="AR2" s="88"/>
+      <c r="AS2" s="88"/>
+      <c r="AT2" s="88"/>
+      <c r="AU2" s="88"/>
+      <c r="AV2" s="88"/>
       <c r="AW2" s="1"/>
-      <c r="AX2" s="49" t="s">
+      <c r="AX2" s="89" t="s">
         <v>15</v>
       </c>
-      <c r="AY2" s="49"/>
-      <c r="AZ2" s="49"/>
-      <c r="BA2" s="49"/>
-      <c r="BB2" s="49"/>
-      <c r="BC2" s="49"/>
-      <c r="BD2" s="50"/>
+      <c r="AY2" s="89"/>
+      <c r="AZ2" s="89"/>
+      <c r="BA2" s="89"/>
+      <c r="BB2" s="89"/>
+      <c r="BC2" s="89"/>
+      <c r="BD2" s="90"/>
       <c r="BE2" s="1"/>
-      <c r="BF2" s="49" t="s">
+      <c r="BF2" s="89" t="s">
         <v>16</v>
       </c>
-      <c r="BG2" s="49"/>
-      <c r="BH2" s="49"/>
-      <c r="BI2" s="49"/>
-      <c r="BJ2" s="49"/>
-      <c r="BK2" s="50"/>
+      <c r="BG2" s="89"/>
+      <c r="BH2" s="89"/>
+      <c r="BI2" s="89"/>
+      <c r="BJ2" s="89"/>
+      <c r="BK2" s="90"/>
       <c r="BL2" s="2"/>
       <c r="BM2" s="1"/>
-      <c r="BN2" s="39" t="s">
+      <c r="BN2" s="88" t="s">
         <v>17</v>
       </c>
-      <c r="BO2" s="39"/>
-      <c r="BP2" s="39"/>
-      <c r="BQ2" s="39"/>
-      <c r="BR2" s="39"/>
-      <c r="BS2" s="39"/>
-      <c r="BT2" s="39"/>
+      <c r="BO2" s="88"/>
+      <c r="BP2" s="88"/>
+      <c r="BQ2" s="88"/>
+      <c r="BR2" s="88"/>
+      <c r="BS2" s="88"/>
+      <c r="BT2" s="88"/>
       <c r="BU2" s="1"/>
-      <c r="BV2" s="39" t="s">
+      <c r="BV2" s="88" t="s">
         <v>18</v>
       </c>
-      <c r="BW2" s="39"/>
-      <c r="BX2" s="39"/>
-      <c r="BY2" s="39"/>
-      <c r="BZ2" s="39"/>
-      <c r="CA2" s="39"/>
-      <c r="CB2" s="39"/>
+      <c r="BW2" s="88"/>
+      <c r="BX2" s="88"/>
+      <c r="BY2" s="88"/>
+      <c r="BZ2" s="88"/>
+      <c r="CA2" s="88"/>
+      <c r="CB2" s="88"/>
       <c r="CC2" s="1"/>
-      <c r="CD2" s="39" t="s">
+      <c r="CD2" s="88" t="s">
         <v>19</v>
       </c>
-      <c r="CE2" s="39"/>
-      <c r="CF2" s="39"/>
-      <c r="CG2" s="39"/>
-      <c r="CH2" s="39"/>
-      <c r="CI2" s="39"/>
-      <c r="CJ2" s="39"/>
+      <c r="CE2" s="88"/>
+      <c r="CF2" s="88"/>
+      <c r="CG2" s="88"/>
+      <c r="CH2" s="88"/>
+      <c r="CI2" s="88"/>
+      <c r="CJ2" s="88"/>
       <c r="CK2" s="1"/>
-      <c r="CL2" s="39" t="s">
+      <c r="CL2" s="88" t="s">
         <v>20</v>
       </c>
-      <c r="CM2" s="39"/>
-      <c r="CN2" s="39"/>
-      <c r="CO2" s="39"/>
-      <c r="CP2" s="39"/>
-      <c r="CQ2" s="39"/>
-      <c r="CR2" s="39"/>
+      <c r="CM2" s="88"/>
+      <c r="CN2" s="88"/>
+      <c r="CO2" s="88"/>
+      <c r="CP2" s="88"/>
+      <c r="CQ2" s="88"/>
+      <c r="CR2" s="88"/>
       <c r="CS2" s="1"/>
-      <c r="CT2" s="39" t="s">
+      <c r="CT2" s="88" t="s">
         <v>21</v>
       </c>
-      <c r="CU2" s="39"/>
-      <c r="CV2" s="39"/>
-      <c r="CW2" s="39"/>
-      <c r="CX2" s="39"/>
-      <c r="CY2" s="39"/>
-      <c r="CZ2" s="39"/>
+      <c r="CU2" s="88"/>
+      <c r="CV2" s="88"/>
+      <c r="CW2" s="88"/>
+      <c r="CX2" s="88"/>
+      <c r="CY2" s="88"/>
+      <c r="CZ2" s="88"/>
       <c r="DA2" s="1"/>
-      <c r="DB2" s="39" t="s">
+      <c r="DB2" s="88" t="s">
         <v>22</v>
       </c>
-      <c r="DC2" s="39"/>
-      <c r="DD2" s="39"/>
-      <c r="DE2" s="39"/>
-      <c r="DF2" s="39"/>
-      <c r="DG2" s="39"/>
-      <c r="DH2" s="39"/>
+      <c r="DC2" s="88"/>
+      <c r="DD2" s="88"/>
+      <c r="DE2" s="88"/>
+      <c r="DF2" s="88"/>
+      <c r="DG2" s="88"/>
+      <c r="DH2" s="88"/>
       <c r="DI2" s="1"/>
-      <c r="DJ2" s="39" t="s">
+      <c r="DJ2" s="88" t="s">
         <v>23</v>
       </c>
-      <c r="DK2" s="39"/>
-      <c r="DL2" s="39"/>
-      <c r="DM2" s="39"/>
-      <c r="DN2" s="39"/>
-      <c r="DO2" s="39"/>
-      <c r="DP2" s="39"/>
+      <c r="DK2" s="88"/>
+      <c r="DL2" s="88"/>
+      <c r="DM2" s="88"/>
+      <c r="DN2" s="88"/>
+      <c r="DO2" s="88"/>
+      <c r="DP2" s="88"/>
       <c r="DQ2" s="1"/>
-      <c r="DR2" s="39" t="s">
+      <c r="DR2" s="88" t="s">
         <v>24</v>
       </c>
-      <c r="DS2" s="39"/>
-      <c r="DT2" s="39"/>
-      <c r="DU2" s="39"/>
-      <c r="DV2" s="39"/>
-      <c r="DW2" s="39"/>
-      <c r="DX2" s="39"/>
+      <c r="DS2" s="88"/>
+      <c r="DT2" s="88"/>
+      <c r="DU2" s="88"/>
+      <c r="DV2" s="88"/>
+      <c r="DW2" s="88"/>
+      <c r="DX2" s="88"/>
       <c r="DY2" s="1"/>
-      <c r="DZ2" s="39" t="s">
+      <c r="DZ2" s="88" t="s">
         <v>25</v>
       </c>
-      <c r="EA2" s="39"/>
-      <c r="EB2" s="39"/>
-      <c r="EC2" s="39"/>
-      <c r="ED2" s="39"/>
-      <c r="EE2" s="39"/>
-      <c r="EF2" s="39"/>
+      <c r="EA2" s="88"/>
+      <c r="EB2" s="88"/>
+      <c r="EC2" s="88"/>
+      <c r="ED2" s="88"/>
+      <c r="EE2" s="88"/>
+      <c r="EF2" s="88"/>
       <c r="EG2" s="1"/>
-      <c r="EH2" s="39" t="s">
+      <c r="EH2" s="88" t="s">
         <v>26</v>
       </c>
-      <c r="EI2" s="39"/>
-      <c r="EJ2" s="39"/>
-      <c r="EK2" s="39"/>
-      <c r="EL2" s="39"/>
-      <c r="EM2" s="39"/>
-      <c r="EN2" s="39"/>
+      <c r="EI2" s="88"/>
+      <c r="EJ2" s="88"/>
+      <c r="EK2" s="88"/>
+      <c r="EL2" s="88"/>
+      <c r="EM2" s="88"/>
+      <c r="EN2" s="88"/>
       <c r="EO2" s="1"/>
-      <c r="EP2" s="39" t="s">
+      <c r="EP2" s="88" t="s">
         <v>27</v>
       </c>
-      <c r="EQ2" s="39"/>
-      <c r="ER2" s="39"/>
-      <c r="ES2" s="39"/>
-      <c r="ET2" s="39"/>
-      <c r="EU2" s="39"/>
-      <c r="EV2" s="39"/>
+      <c r="EQ2" s="88"/>
+      <c r="ER2" s="88"/>
+      <c r="ES2" s="88"/>
+      <c r="ET2" s="88"/>
+      <c r="EU2" s="88"/>
+      <c r="EV2" s="88"/>
       <c r="EW2" s="1"/>
-      <c r="EX2" s="39" t="s">
+      <c r="EX2" s="88" t="s">
         <v>28</v>
       </c>
-      <c r="EY2" s="39"/>
-      <c r="EZ2" s="39"/>
-      <c r="FA2" s="39"/>
-      <c r="FB2" s="39"/>
-      <c r="FC2" s="39"/>
-      <c r="FD2" s="39"/>
+      <c r="EY2" s="88"/>
+      <c r="EZ2" s="88"/>
+      <c r="FA2" s="88"/>
+      <c r="FB2" s="88"/>
+      <c r="FC2" s="88"/>
+      <c r="FD2" s="88"/>
       <c r="FE2" s="1"/>
-      <c r="FF2" s="39" t="s">
+      <c r="FF2" s="88" t="s">
         <v>29</v>
       </c>
-      <c r="FG2" s="39"/>
-      <c r="FH2" s="39"/>
-      <c r="FI2" s="39"/>
-      <c r="FJ2" s="39"/>
-      <c r="FK2" s="39"/>
-      <c r="FL2" s="39"/>
+      <c r="FG2" s="88"/>
+      <c r="FH2" s="88"/>
+      <c r="FI2" s="88"/>
+      <c r="FJ2" s="88"/>
+      <c r="FK2" s="88"/>
+      <c r="FL2" s="88"/>
       <c r="FM2" s="1"/>
-      <c r="FN2" s="39" t="s">
+      <c r="FN2" s="88" t="s">
         <v>30</v>
       </c>
-      <c r="FO2" s="39"/>
-      <c r="FP2" s="39"/>
-      <c r="FQ2" s="39"/>
-      <c r="FR2" s="39"/>
-      <c r="FS2" s="39"/>
-      <c r="FT2" s="39"/>
+      <c r="FO2" s="88"/>
+      <c r="FP2" s="88"/>
+      <c r="FQ2" s="88"/>
+      <c r="FR2" s="88"/>
+      <c r="FS2" s="88"/>
+      <c r="FT2" s="88"/>
       <c r="FU2" s="1"/>
     </row>
     <row r="3" spans="1:177" x14ac:dyDescent="0.2">
-      <c r="A3" s="45"/>
+      <c r="A3" s="84"/>
       <c r="B3" s="11" t="s">
         <v>32</v>
       </c>
@@ -9725,181 +9789,489 @@
       <c r="A20" s="5">
         <v>45267</v>
       </c>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="34"/>
-      <c r="H20" s="35"/>
+      <c r="B20" s="6">
+        <v>727762</v>
+      </c>
+      <c r="C20" s="6">
+        <v>1097415</v>
+      </c>
+      <c r="D20" s="6">
+        <v>-369653</v>
+      </c>
+      <c r="E20" s="6">
+        <v>-8224660000</v>
+      </c>
+      <c r="F20" s="100">
+        <v>67492301</v>
+      </c>
+      <c r="G20" s="40">
+        <v>2.7042743734577962E-2</v>
+      </c>
+      <c r="H20" s="41">
+        <v>-3.6363636363636397E-2</v>
+      </c>
       <c r="I20" s="1"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="6"/>
-      <c r="M20" s="6"/>
-      <c r="N20" s="6"/>
-      <c r="O20" s="34"/>
-      <c r="P20" s="35"/>
+      <c r="J20" s="6">
+        <v>1651000</v>
+      </c>
+      <c r="K20" s="6">
+        <v>804992</v>
+      </c>
+      <c r="L20" s="6">
+        <v>846008</v>
+      </c>
+      <c r="M20" s="6">
+        <v>27628170000</v>
+      </c>
+      <c r="N20" s="100">
+        <v>44258101</v>
+      </c>
+      <c r="O20" s="42">
+        <v>5.5492484867346661E-2</v>
+      </c>
+      <c r="P20" s="43">
+        <v>-2.2831050228310501E-2</v>
+      </c>
       <c r="Q20" s="1"/>
-      <c r="R20" s="6"/>
-      <c r="S20" s="6"/>
-      <c r="T20" s="6"/>
-      <c r="U20" s="6"/>
-      <c r="V20" s="6"/>
-      <c r="W20" s="34"/>
-      <c r="X20" s="35"/>
+      <c r="R20" s="6">
+        <v>792960</v>
+      </c>
+      <c r="S20" s="6">
+        <v>243562</v>
+      </c>
+      <c r="T20" s="6">
+        <v>549398</v>
+      </c>
+      <c r="U20" s="6">
+        <v>45601610000</v>
+      </c>
+      <c r="V20" s="6">
+        <v>2403460</v>
+      </c>
+      <c r="W20" s="44">
+        <v>0.43126242999675468</v>
+      </c>
+      <c r="X20" s="45">
+        <v>-5.8685446009389668E-3</v>
+      </c>
       <c r="Y20" s="1"/>
-      <c r="Z20" s="6"/>
-      <c r="AA20" s="6"/>
-      <c r="AB20" s="6"/>
-      <c r="AC20" s="6"/>
-      <c r="AD20" s="6"/>
-      <c r="AE20" s="34"/>
-      <c r="AF20" s="35"/>
+      <c r="Z20" s="6">
+        <v>2641000</v>
+      </c>
+      <c r="AA20" s="6">
+        <v>3895990</v>
+      </c>
+      <c r="AB20" s="6">
+        <v>-1254990</v>
+      </c>
+      <c r="AC20" s="6">
+        <v>-24158040000</v>
+      </c>
+      <c r="AD20" s="6">
+        <v>22918000</v>
+      </c>
+      <c r="AE20" s="46">
+        <v>0.28523387730168426</v>
+      </c>
+      <c r="AF20" s="47">
+        <v>1.2886597938144331E-2</v>
+      </c>
       <c r="AG20" s="1"/>
-      <c r="AH20" s="6"/>
-      <c r="AI20" s="6"/>
-      <c r="AJ20" s="6"/>
-      <c r="AK20" s="6"/>
-      <c r="AL20" s="6"/>
-      <c r="AM20" s="34"/>
-      <c r="AN20" s="35"/>
+      <c r="AH20" s="6">
+        <v>548800</v>
+      </c>
+      <c r="AI20" s="6">
+        <v>3855025</v>
+      </c>
+      <c r="AJ20" s="6">
+        <v>-3306225</v>
+      </c>
+      <c r="AK20" s="6">
+        <v>-94209490000</v>
+      </c>
+      <c r="AL20" s="6">
+        <v>29322200</v>
+      </c>
+      <c r="AM20" s="48">
+        <v>0.15018740067252798</v>
+      </c>
+      <c r="AN20" s="49">
+        <v>8.8339222614840993E-3</v>
+      </c>
       <c r="AO20" s="1"/>
-      <c r="AP20" s="6"/>
-      <c r="AQ20" s="6"/>
-      <c r="AR20" s="6"/>
-      <c r="AS20" s="6"/>
-      <c r="AT20" s="6"/>
-      <c r="AU20" s="34"/>
-      <c r="AV20" s="35"/>
+      <c r="AP20" s="6">
+        <v>4484850</v>
+      </c>
+      <c r="AQ20" s="6">
+        <v>6005598</v>
+      </c>
+      <c r="AR20" s="6">
+        <v>-1520748</v>
+      </c>
+      <c r="AS20" s="6">
+        <v>-42112220000</v>
+      </c>
+      <c r="AT20" s="6">
+        <v>50275900</v>
+      </c>
+      <c r="AU20" s="50">
+        <v>0.2086575874325472</v>
+      </c>
+      <c r="AV20" s="51">
+        <v>-1.8115942028984477E-3</v>
+      </c>
       <c r="AW20" s="1"/>
-      <c r="AX20" s="6"/>
-      <c r="AY20" s="6"/>
-      <c r="AZ20" s="6"/>
-      <c r="BA20" s="6"/>
-      <c r="BB20" s="6"/>
-      <c r="BC20" s="34"/>
-      <c r="BD20" s="35"/>
+      <c r="AX20" s="6">
+        <v>30970</v>
+      </c>
+      <c r="AY20" s="6">
+        <v>563336</v>
+      </c>
+      <c r="AZ20" s="6">
+        <v>-532366</v>
+      </c>
+      <c r="BA20" s="6">
+        <v>-12356160000</v>
+      </c>
+      <c r="BB20" s="6">
+        <v>15719200</v>
+      </c>
+      <c r="BC20" s="52">
+        <v>3.7807649244236345E-2</v>
+      </c>
+      <c r="BD20" s="53">
+        <v>-2.5751072961373297E-2</v>
+      </c>
       <c r="BE20" s="1"/>
-      <c r="BF20" s="6"/>
-      <c r="BG20" s="6"/>
-      <c r="BH20" s="6"/>
-      <c r="BI20" s="6"/>
-      <c r="BJ20" s="6"/>
-      <c r="BK20" s="34"/>
-      <c r="BL20" s="35"/>
+      <c r="BF20" s="6">
+        <v>1602300</v>
+      </c>
+      <c r="BG20" s="6">
+        <v>2020800</v>
+      </c>
+      <c r="BH20" s="6">
+        <v>-418500</v>
+      </c>
+      <c r="BI20" s="6">
+        <v>-16993520000</v>
+      </c>
+      <c r="BJ20" s="6">
+        <v>11560000</v>
+      </c>
+      <c r="BK20" s="54">
+        <v>0.31341695501730105</v>
+      </c>
+      <c r="BL20" s="55">
+        <v>-4.895960832313237E-3</v>
+      </c>
       <c r="BM20" s="1"/>
-      <c r="BN20" s="6"/>
-      <c r="BO20" s="6"/>
-      <c r="BP20" s="6"/>
-      <c r="BQ20" s="6"/>
-      <c r="BR20" s="6"/>
-      <c r="BS20" s="34"/>
-      <c r="BT20" s="35"/>
+      <c r="BN20" s="6">
+        <v>514514</v>
+      </c>
+      <c r="BO20" s="6">
+        <v>1730200</v>
+      </c>
+      <c r="BP20" s="6">
+        <v>-1215686</v>
+      </c>
+      <c r="BQ20" s="6">
+        <v>-27762660000</v>
+      </c>
+      <c r="BR20" s="6">
+        <v>5052900</v>
+      </c>
+      <c r="BS20" s="56">
+        <v>0.44424271210591937</v>
+      </c>
+      <c r="BT20" s="57">
+        <v>-6.5789473684209898E-3</v>
+      </c>
       <c r="BU20" s="1"/>
-      <c r="BV20" s="6"/>
-      <c r="BW20" s="6"/>
-      <c r="BX20" s="6"/>
-      <c r="BY20" s="6"/>
-      <c r="BZ20" s="6"/>
-      <c r="CA20" s="34"/>
-      <c r="CB20" s="35"/>
+      <c r="BV20" s="6">
+        <v>99450</v>
+      </c>
+      <c r="BW20" s="6">
+        <v>134341</v>
+      </c>
+      <c r="BX20" s="6">
+        <v>-34891</v>
+      </c>
+      <c r="BY20" s="6">
+        <v>-3406830000</v>
+      </c>
+      <c r="BZ20" s="6">
+        <v>397400</v>
+      </c>
+      <c r="CA20" s="58">
+        <v>0.58830145948666335</v>
+      </c>
+      <c r="CB20" s="59">
+        <v>1.9665683382497821E-3</v>
+      </c>
       <c r="CC20" s="1"/>
-      <c r="CD20" s="6"/>
-      <c r="CE20" s="6"/>
-      <c r="CF20" s="6"/>
-      <c r="CG20" s="6"/>
-      <c r="CH20" s="6"/>
-      <c r="CI20" s="34"/>
-      <c r="CJ20" s="35"/>
+      <c r="CD20" s="6">
+        <v>1226742</v>
+      </c>
+      <c r="CE20" s="6">
+        <v>6529100</v>
+      </c>
+      <c r="CF20" s="6">
+        <v>-5302358</v>
+      </c>
+      <c r="CG20" s="6">
+        <v>-210801490000</v>
+      </c>
+      <c r="CH20" s="6">
+        <v>11365000</v>
+      </c>
+      <c r="CI20" s="60">
+        <v>0.68243220413550376</v>
+      </c>
+      <c r="CJ20" s="61">
+        <v>-1.8891687657430729E-2</v>
+      </c>
       <c r="CK20" s="1"/>
-      <c r="CL20" s="6"/>
-      <c r="CM20" s="6"/>
-      <c r="CN20" s="6"/>
-      <c r="CO20" s="6"/>
-      <c r="CP20" s="6"/>
-      <c r="CQ20" s="34"/>
-      <c r="CR20" s="35"/>
+      <c r="CL20" s="6">
+        <v>664700</v>
+      </c>
+      <c r="CM20" s="6">
+        <v>1067530</v>
+      </c>
+      <c r="CN20" s="6">
+        <v>-402830</v>
+      </c>
+      <c r="CO20" s="6">
+        <v>-8531630000</v>
+      </c>
+      <c r="CP20" s="6">
+        <v>36084500</v>
+      </c>
+      <c r="CQ20" s="62">
+        <v>4.8004822014992586E-2</v>
+      </c>
+      <c r="CR20" s="63">
+        <v>-4.3902439024390172E-2</v>
+      </c>
       <c r="CS20" s="1"/>
-      <c r="CT20" s="6"/>
-      <c r="CU20" s="6"/>
-      <c r="CV20" s="6"/>
-      <c r="CW20" s="6"/>
-      <c r="CX20" s="6"/>
-      <c r="CY20" s="34"/>
-      <c r="CZ20" s="35"/>
+      <c r="CT20" s="6">
+        <v>281717</v>
+      </c>
+      <c r="CU20" s="6">
+        <v>759500</v>
+      </c>
+      <c r="CV20" s="6">
+        <v>-477783</v>
+      </c>
+      <c r="CW20" s="6">
+        <v>-13528720000</v>
+      </c>
+      <c r="CX20" s="6">
+        <v>22262724</v>
+      </c>
+      <c r="CY20" s="64">
+        <v>4.6769523801310206E-2</v>
+      </c>
+      <c r="CZ20" s="65">
+        <v>-1.04712041884817E-2</v>
+      </c>
       <c r="DA20" s="1"/>
-      <c r="DB20" s="6"/>
-      <c r="DC20" s="6"/>
-      <c r="DD20" s="6"/>
-      <c r="DE20" s="6"/>
-      <c r="DF20" s="6"/>
-      <c r="DG20" s="34"/>
-      <c r="DH20" s="35"/>
+      <c r="DB20" s="6">
+        <v>801173</v>
+      </c>
+      <c r="DC20" s="6">
+        <v>132632</v>
+      </c>
+      <c r="DD20" s="6">
+        <v>668541</v>
+      </c>
+      <c r="DE20" s="99">
+        <v>11857110000</v>
+      </c>
+      <c r="DF20" s="6">
+        <v>46674900</v>
+      </c>
+      <c r="DG20" s="66">
+        <v>2.0006577410985348E-2</v>
+      </c>
+      <c r="DH20" s="67">
+        <v>-4.2857142857142858E-2</v>
+      </c>
       <c r="DI20" s="1"/>
-      <c r="DJ20" s="6"/>
-      <c r="DK20" s="6"/>
-      <c r="DL20" s="6"/>
-      <c r="DM20" s="6"/>
-      <c r="DN20" s="6"/>
-      <c r="DO20" s="34"/>
-      <c r="DP20" s="35"/>
+      <c r="DJ20" s="6">
+        <v>780800</v>
+      </c>
+      <c r="DK20" s="6">
+        <v>174530</v>
+      </c>
+      <c r="DL20" s="6">
+        <v>606270</v>
+      </c>
+      <c r="DM20" s="99">
+        <v>19497790000</v>
+      </c>
+      <c r="DN20" s="99">
+        <v>12707700</v>
+      </c>
+      <c r="DO20" s="68">
+        <v>7.5177254735317958E-2</v>
+      </c>
+      <c r="DP20" s="69">
+        <v>-2.6397515527950131E-2</v>
+      </c>
       <c r="DQ20" s="1"/>
-      <c r="DR20" s="6"/>
-      <c r="DS20" s="6"/>
-      <c r="DT20" s="6"/>
-      <c r="DU20" s="6"/>
-      <c r="DV20" s="6"/>
-      <c r="DW20" s="34"/>
-      <c r="DX20" s="35"/>
+      <c r="DR20" s="6">
+        <v>154000</v>
+      </c>
+      <c r="DS20" s="6">
+        <v>43200</v>
+      </c>
+      <c r="DT20" s="6">
+        <v>110800</v>
+      </c>
+      <c r="DU20" s="6">
+        <v>7738360000</v>
+      </c>
+      <c r="DV20" s="6">
+        <v>949000</v>
+      </c>
+      <c r="DW20" s="70">
+        <v>0.20779768177028451</v>
+      </c>
+      <c r="DX20" s="71">
+        <v>-1.4204545454544646E-3</v>
+      </c>
       <c r="DY20" s="1"/>
-      <c r="DZ20" s="6"/>
-      <c r="EA20" s="6"/>
-      <c r="EB20" s="6"/>
-      <c r="EC20" s="6"/>
-      <c r="ED20" s="6"/>
-      <c r="EE20" s="34"/>
-      <c r="EF20" s="35"/>
+      <c r="DZ20" s="6">
+        <v>1000</v>
+      </c>
+      <c r="EA20" s="6">
+        <v>175123</v>
+      </c>
+      <c r="EB20" s="6">
+        <v>-174123</v>
+      </c>
+      <c r="EC20" s="6">
+        <v>-6387760000</v>
+      </c>
+      <c r="ED20" s="6">
+        <v>4552100</v>
+      </c>
+      <c r="EE20" s="72">
+        <v>3.869049449704532E-2</v>
+      </c>
+      <c r="EF20" s="73">
+        <v>-2.0380434782608696E-2</v>
+      </c>
       <c r="EG20" s="1"/>
-      <c r="EH20" s="6"/>
-      <c r="EI20" s="6"/>
-      <c r="EJ20" s="6"/>
-      <c r="EK20" s="6"/>
-      <c r="EL20" s="6"/>
-      <c r="EM20" s="34"/>
-      <c r="EN20" s="35"/>
+      <c r="EH20" s="6">
+        <v>72200</v>
+      </c>
+      <c r="EI20" s="6">
+        <v>74100</v>
+      </c>
+      <c r="EJ20" s="6">
+        <v>-1900</v>
+      </c>
+      <c r="EK20" s="6">
+        <v>-97530000</v>
+      </c>
+      <c r="EL20" s="6">
+        <v>2756100</v>
+      </c>
+      <c r="EM20" s="74">
+        <v>5.3082253909509818E-2</v>
+      </c>
+      <c r="EN20" s="75">
+        <v>-6.0882800608826702E-3</v>
+      </c>
       <c r="EO20" s="1"/>
-      <c r="EP20" s="6"/>
-      <c r="EQ20" s="6"/>
-      <c r="ER20" s="6"/>
-      <c r="ES20" s="6"/>
-      <c r="ET20" s="6"/>
-      <c r="EU20" s="34"/>
-      <c r="EV20" s="35"/>
+      <c r="EP20" s="6">
+        <v>615200</v>
+      </c>
+      <c r="EQ20" s="6">
+        <v>452600</v>
+      </c>
+      <c r="ER20" s="6">
+        <v>162600</v>
+      </c>
+      <c r="ES20" s="6">
+        <v>3964740000</v>
+      </c>
+      <c r="ET20" s="6">
+        <v>17717600</v>
+      </c>
+      <c r="EU20" s="76">
+        <v>6.0267756355262561E-2</v>
+      </c>
+      <c r="EV20" s="77">
+        <v>-1.632653061224484E-2</v>
+      </c>
       <c r="EW20" s="1"/>
-      <c r="EX20" s="6"/>
-      <c r="EY20" s="6"/>
-      <c r="EZ20" s="6"/>
-      <c r="FA20" s="6"/>
-      <c r="FB20" s="6"/>
-      <c r="FC20" s="34"/>
-      <c r="FD20" s="35"/>
+      <c r="EX20" s="6">
+        <v>204100</v>
+      </c>
+      <c r="EY20" s="6">
+        <v>1104300</v>
+      </c>
+      <c r="EZ20" s="6">
+        <v>-900200</v>
+      </c>
+      <c r="FA20" s="6">
+        <v>-21241180000</v>
+      </c>
+      <c r="FB20" s="6">
+        <v>42267200</v>
+      </c>
+      <c r="FC20" s="78">
+        <v>3.0955445357156375E-2</v>
+      </c>
+      <c r="FD20" s="79">
+        <v>-2.3504273504273535E-2</v>
+      </c>
       <c r="FE20" s="1"/>
-      <c r="FF20" s="6"/>
-      <c r="FG20" s="6"/>
-      <c r="FH20" s="6"/>
-      <c r="FI20" s="6"/>
-      <c r="FJ20" s="6"/>
-      <c r="FK20" s="34"/>
-      <c r="FL20" s="35"/>
+      <c r="FF20" s="6">
+        <v>323800</v>
+      </c>
+      <c r="FG20" s="6">
+        <v>49200</v>
+      </c>
+      <c r="FH20" s="6">
+        <v>274600</v>
+      </c>
+      <c r="FI20" s="6">
+        <v>26676250000</v>
+      </c>
+      <c r="FJ20" s="6">
+        <v>4001300</v>
+      </c>
+      <c r="FK20" s="80">
+        <v>9.3219703596331194E-2</v>
+      </c>
+      <c r="FL20" s="81">
+        <v>-8.2304526748970906E-3</v>
+      </c>
       <c r="FM20" s="1"/>
-      <c r="FN20" s="6"/>
-      <c r="FO20" s="6"/>
-      <c r="FP20" s="6"/>
-      <c r="FQ20" s="6"/>
-      <c r="FR20" s="6"/>
-      <c r="FS20" s="34"/>
-      <c r="FT20" s="35"/>
+      <c r="FN20" s="6">
+        <v>617900</v>
+      </c>
+      <c r="FO20" s="6">
+        <v>10800</v>
+      </c>
+      <c r="FP20" s="6">
+        <v>607100</v>
+      </c>
+      <c r="FQ20" s="6">
+        <v>45683440000</v>
+      </c>
+      <c r="FR20" s="6">
+        <v>1504300</v>
+      </c>
+      <c r="FS20" s="82">
+        <v>0.4179352522768065</v>
+      </c>
+      <c r="FT20" s="83">
+        <v>-2.6385224274406709E-3</v>
+      </c>
       <c r="FU20" s="1"/>
     </row>
     <row r="21" spans="1:177" x14ac:dyDescent="0.2">
@@ -11985,23 +12357,6 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="BF1:CB1"/>
-    <mergeCell ref="CD1:DP1"/>
-    <mergeCell ref="DR1:EF1"/>
-    <mergeCell ref="DZ2:EF2"/>
-    <mergeCell ref="CT2:CZ2"/>
-    <mergeCell ref="DB2:DH2"/>
-    <mergeCell ref="DJ2:DP2"/>
-    <mergeCell ref="AX2:BD2"/>
-    <mergeCell ref="BF2:BK2"/>
-    <mergeCell ref="BN2:BT2"/>
-    <mergeCell ref="EX1:FD1"/>
-    <mergeCell ref="CL2:CR2"/>
-    <mergeCell ref="DR2:DX2"/>
-    <mergeCell ref="EH1:EV1"/>
-    <mergeCell ref="FF1:FL1"/>
-    <mergeCell ref="BV2:CB2"/>
     <mergeCell ref="FN1:FT1"/>
     <mergeCell ref="J2:P2"/>
     <mergeCell ref="R2:X2"/>
@@ -12016,6 +12371,23 @@
     <mergeCell ref="FN2:FT2"/>
     <mergeCell ref="CD2:CJ2"/>
     <mergeCell ref="EH2:EN2"/>
+    <mergeCell ref="EX1:FD1"/>
+    <mergeCell ref="CL2:CR2"/>
+    <mergeCell ref="DR2:DX2"/>
+    <mergeCell ref="EH1:EV1"/>
+    <mergeCell ref="FF1:FL1"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="BF1:CB1"/>
+    <mergeCell ref="CD1:DP1"/>
+    <mergeCell ref="DR1:EF1"/>
+    <mergeCell ref="DZ2:EF2"/>
+    <mergeCell ref="CT2:CZ2"/>
+    <mergeCell ref="DB2:DH2"/>
+    <mergeCell ref="DJ2:DP2"/>
+    <mergeCell ref="AX2:BD2"/>
+    <mergeCell ref="BF2:BK2"/>
+    <mergeCell ref="BN2:BT2"/>
+    <mergeCell ref="BV2:CB2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -12039,18 +12411,18 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="13"/>
-      <c r="B1" s="51" t="s">
+      <c r="B1" s="97" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
+      <c r="C1" s="97"/>
+      <c r="D1" s="97"/>
+      <c r="E1" s="97"/>
+      <c r="F1" s="97"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="97"/>
+      <c r="I1" s="97"/>
+      <c r="J1" s="97"/>
+      <c r="K1" s="97"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
@@ -12714,10 +13086,10 @@
       <c r="F26" s="12"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" s="52" t="s">
+      <c r="A27" s="98" t="s">
         <v>57</v>
       </c>
-      <c r="B27" s="52"/>
+      <c r="B27" s="98"/>
       <c r="C27" s="25">
         <f>SUM(C3:C25)</f>
         <v>16.700000000000003</v>
@@ -12728,10 +13100,10 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A28" s="52" t="s">
+      <c r="A28" s="98" t="s">
         <v>58</v>
       </c>
-      <c r="B28" s="52"/>
+      <c r="B28" s="98"/>
       <c r="G28" s="6">
         <f>AVERAGE(G3:G25)</f>
         <v>835451092.93333328</v>
@@ -12739,10 +13111,10 @@
       <c r="H28" s="6"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" s="52" t="s">
+      <c r="A29" s="98" t="s">
         <v>59</v>
       </c>
-      <c r="B29" s="52"/>
+      <c r="B29" s="98"/>
       <c r="E29" s="10">
         <f>AVERAGE(E3:E25)</f>
         <v>1.4712500000000002E-2</v>
@@ -12750,10 +13122,10 @@
       <c r="F29" s="10"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A30" s="52" t="s">
+      <c r="A30" s="98" t="s">
         <v>75</v>
       </c>
-      <c r="B30" s="52"/>
+      <c r="B30" s="98"/>
       <c r="F30" s="6">
         <f>SUM(F3:F25)</f>
         <v>-4389127666595.1631</v>

</xml_diff>